<commit_message>
Annotatie Type (reworked) Datumbepaling Type Kleur Type
</commit_message>
<xml_diff>
--- a/admin/rdm/Digipolis_Lookup_RDM_Cleaning.xlsx
+++ b/admin/rdm/Digipolis_Lookup_RDM_Cleaning.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="24" yWindow="456" windowWidth="28404" windowHeight="17040" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="24" yWindow="456" windowWidth="28404" windowHeight="17040" firstSheet="7" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="CSV &lt;-&gt; RDM" sheetId="25" r:id="rId1"/>
@@ -290,7 +290,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1732" uniqueCount="1350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1919" uniqueCount="1393">
   <si>
     <t>code</t>
   </si>
@@ -4285,61 +4285,190 @@
     <t>AAT ID</t>
   </si>
   <si>
-    <t>Digipolis Thesauri\Objectkenmerken\Titel Type\published titles</t>
-  </si>
-  <si>
-    <t>Digipolis Thesauri\Objectkenmerken\Titel Type\incipits</t>
-  </si>
-  <si>
-    <t>Digipolis Thesauri\Objectkenmerken\Titel Type\collective titles</t>
-  </si>
-  <si>
-    <t>Digipolis Thesauri\Objectkenmerken\Titel Type\titles proper</t>
-  </si>
-  <si>
-    <t>Digipolis Thesauri\Objectkenmerken\Taal Type\English (language)</t>
-  </si>
-  <si>
-    <t>Digipolis Thesauri\Objectkenmerken\Taal Type\Dutch (language)</t>
-  </si>
-  <si>
-    <t>Digipolis Thesauri\Objectkenmerken\Taal Type\French (language)</t>
-  </si>
-  <si>
-    <t>Digipolis Thesauri\Objectkenmerken\Taal Type\German (language)</t>
-  </si>
-  <si>
-    <t>Digipolis Thesauri\Objectkenmerken\Taal Type\Ancient Greek (language)</t>
-  </si>
-  <si>
-    <t>Digipolis Thesauri\Objectkenmerken\Taal Type\Greek (language)</t>
-  </si>
-  <si>
-    <t>Digipolis Thesauri\Objectkenmerken\Taal Type\Hebrew (language)</t>
-  </si>
-  <si>
-    <t>Digipolis Thesauri\Objectkenmerken\Taal Type\Italian (language)</t>
-  </si>
-  <si>
-    <t>Digipolis Thesauri\Objectkenmerken\Taal Type\Latin (language)</t>
-  </si>
-  <si>
-    <t>Digipolis Thesauri\Objectkenmerken\Taal Type\Norwegian (language)</t>
-  </si>
-  <si>
-    <t>Digipolis Thesauri\Objectkenmerken\Taal Type\Portuguese (language)</t>
-  </si>
-  <si>
-    <t>Digipolis Thesauri\Objectkenmerken\Taal Type\Spanish (language)</t>
-  </si>
-  <si>
-    <t>Digipolis Thesauri\Objectkenmerken\Taal Type\Swedish (language)</t>
-  </si>
-  <si>
-    <t>Digipolis Thesauri\Objectkenmerken\Annotatie Type\remarks</t>
-  </si>
-  <si>
-    <t>Digipolis Thesauri\Objectkenmerken\Annotatie Type\descriptive note</t>
+    <t>inscription description</t>
+  </si>
+  <si>
+    <t>groepsbeschrijving</t>
+  </si>
+  <si>
+    <t>gerelateerde kunstwerken</t>
+  </si>
+  <si>
+    <t>circa</t>
+  </si>
+  <si>
+    <t>centuries</t>
+  </si>
+  <si>
+    <t>onzeker</t>
+  </si>
+  <si>
+    <t>datum voor</t>
+  </si>
+  <si>
+    <t>datum na</t>
+  </si>
+  <si>
+    <t>beige (color)</t>
+  </si>
+  <si>
+    <t>blue (color)</t>
+  </si>
+  <si>
+    <t>brown (color)</t>
+  </si>
+  <si>
+    <t>bronze (color)</t>
+  </si>
+  <si>
+    <t>yellow (color)</t>
+  </si>
+  <si>
+    <t>green (color)</t>
+  </si>
+  <si>
+    <t>cream (color)</t>
+  </si>
+  <si>
+    <t>ivory (color)</t>
+  </si>
+  <si>
+    <t>gray (color)</t>
+  </si>
+  <si>
+    <t>ocher (color)</t>
+  </si>
+  <si>
+    <t>orange (color)</t>
+  </si>
+  <si>
+    <t>gold (color)</t>
+  </si>
+  <si>
+    <t>purple (color)</t>
+  </si>
+  <si>
+    <t>red (color)</t>
+  </si>
+  <si>
+    <t>pink (color)</t>
+  </si>
+  <si>
+    <t>sepia (color)</t>
+  </si>
+  <si>
+    <t>white (color)</t>
+  </si>
+  <si>
+    <t>silver (color)</t>
+  </si>
+  <si>
+    <t>black (color)</t>
+  </si>
+  <si>
+    <t>thesaurus</t>
+  </si>
+  <si>
+    <t>Digipolis Thesauri\Objectkenmerken\Annotatie Type\</t>
+  </si>
+  <si>
+    <t>remarks</t>
+  </si>
+  <si>
+    <t>Digipolis Thesauri\Objectkenmerken\Beschrijving Type\</t>
+  </si>
+  <si>
+    <t>Digipolis Thesaurus\Objectkenmerken\Annotatie Type\</t>
+  </si>
+  <si>
+    <t>condition/examination description</t>
+  </si>
+  <si>
+    <t>descriptive note</t>
+  </si>
+  <si>
+    <t>detailbeschrijving</t>
+  </si>
+  <si>
+    <t>provenance description</t>
+  </si>
+  <si>
+    <t>temporary location</t>
+  </si>
+  <si>
+    <t>related artwork</t>
+  </si>
+  <si>
+    <t>Digipolis Thesauri\Objectkenmerken\Datumbepaling Type\</t>
+  </si>
+  <si>
+    <t>Digipolis Thesauri\Objectkenmerken\Kleur Type\</t>
+  </si>
+  <si>
+    <t>Digipolis Thesauri\Objectkenmerken\Taal Type\</t>
+  </si>
+  <si>
+    <t>Dutch (language)</t>
+  </si>
+  <si>
+    <t>English (language)</t>
+  </si>
+  <si>
+    <t>French (language)</t>
+  </si>
+  <si>
+    <t>German (language)</t>
+  </si>
+  <si>
+    <t>Ancient Greek (language)</t>
+  </si>
+  <si>
+    <t>Greek (language)</t>
+  </si>
+  <si>
+    <t>Hebrew (language)</t>
+  </si>
+  <si>
+    <t>Italian (language)</t>
+  </si>
+  <si>
+    <t>Latin (language)</t>
+  </si>
+  <si>
+    <t>Norwegian (language)</t>
+  </si>
+  <si>
+    <t>Portuguese (language)</t>
+  </si>
+  <si>
+    <t>Spanish (language)</t>
+  </si>
+  <si>
+    <t>Swedish (language)</t>
+  </si>
+  <si>
+    <t>published titles</t>
+  </si>
+  <si>
+    <t>incipits</t>
+  </si>
+  <si>
+    <t>collective titles</t>
+  </si>
+  <si>
+    <t>titles proper</t>
+  </si>
+  <si>
+    <t>Digipolis Thesauri\Objectkenmerken\Titel Type\</t>
+  </si>
+  <si>
+    <t>Low German (language)</t>
+  </si>
+  <si>
+    <t>undetermined (language)</t>
+  </si>
+  <si>
+    <t>unidentified (information indicator)</t>
   </si>
 </sst>
 </file>
@@ -5042,14 +5171,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.69921875" customWidth="1"/>
+    <col min="4" max="4" width="22.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -5060,7 +5191,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1157</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1330</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1328</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -5070,6 +5210,9 @@
       <c r="B2" t="s">
         <v>141</v>
       </c>
+      <c r="F2" t="s">
+        <v>1329</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -5078,6 +5221,15 @@
       <c r="B3" t="s">
         <v>143</v>
       </c>
+      <c r="C3" t="s">
+        <v>1369</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1334</v>
+      </c>
+      <c r="E3">
+        <v>300435723</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -5086,6 +5238,15 @@
       <c r="B4" t="s">
         <v>145</v>
       </c>
+      <c r="C4" t="s">
+        <v>1369</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1334</v>
+      </c>
+      <c r="E4">
+        <v>300435723</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -5094,6 +5255,15 @@
       <c r="B5" t="s">
         <v>147</v>
       </c>
+      <c r="C5" t="s">
+        <v>1369</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1335</v>
+      </c>
+      <c r="E5">
+        <v>300379247</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -5102,6 +5272,12 @@
       <c r="B6" t="s">
         <v>149</v>
       </c>
+      <c r="C6" t="s">
+        <v>1369</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1336</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -5110,6 +5286,15 @@
       <c r="B7" t="s">
         <v>151</v>
       </c>
+      <c r="C7" t="s">
+        <v>1369</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1392</v>
+      </c>
+      <c r="E7">
+        <v>300386154</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -5118,6 +5303,12 @@
       <c r="B8" t="s">
         <v>153</v>
       </c>
+      <c r="C8" t="s">
+        <v>1369</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1337</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -5126,6 +5317,12 @@
       <c r="B9" t="s">
         <v>155</v>
       </c>
+      <c r="C9" t="s">
+        <v>1369</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1338</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -5133,6 +5330,15 @@
       </c>
       <c r="B10" t="s">
         <v>157</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1369</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1334</v>
+      </c>
+      <c r="E10">
+        <v>300435723</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -5179,15 +5385,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -5196,7 +5403,7 @@
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5204,10 +5411,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1157</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>1330</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>158</v>
       </c>
@@ -5215,7 +5431,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>160</v>
       </c>
@@ -5230,10 +5446,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C74"/>
+  <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -5242,7 +5458,7 @@
     <col min="2" max="2" width="37" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5250,10 +5466,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1157</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>1330</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>162</v>
       </c>
@@ -5261,7 +5486,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>164</v>
       </c>
@@ -5269,7 +5494,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>166</v>
       </c>
@@ -5277,7 +5502,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>168</v>
       </c>
@@ -5285,7 +5510,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>170</v>
       </c>
@@ -5293,7 +5518,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>172</v>
       </c>
@@ -5301,7 +5526,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>174</v>
       </c>
@@ -5309,7 +5534,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>176</v>
       </c>
@@ -5317,7 +5542,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>178</v>
       </c>
@@ -5325,7 +5550,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>180</v>
       </c>
@@ -5333,7 +5558,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>182</v>
       </c>
@@ -5341,7 +5566,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>184</v>
       </c>
@@ -5349,7 +5574,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>186</v>
       </c>
@@ -5357,7 +5582,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>188</v>
       </c>
@@ -5365,7 +5590,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>190</v>
       </c>
@@ -5836,10 +6061,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -5848,7 +6073,7 @@
     <col min="2" max="2" width="42.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5856,10 +6081,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1157</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>1330</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>303</v>
       </c>
@@ -5867,7 +6101,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>305</v>
       </c>
@@ -5875,7 +6109,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>307</v>
       </c>
@@ -5883,7 +6117,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>309</v>
       </c>
@@ -5891,7 +6125,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>311</v>
       </c>
@@ -5899,7 +6133,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>312</v>
       </c>
@@ -5907,7 +6141,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>314</v>
       </c>
@@ -5915,7 +6149,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>316</v>
       </c>
@@ -5923,7 +6157,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>318</v>
       </c>
@@ -5931,7 +6165,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>320</v>
       </c>
@@ -5939,7 +6173,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>321</v>
       </c>
@@ -5947,7 +6181,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>323</v>
       </c>
@@ -5955,7 +6189,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>324</v>
       </c>
@@ -5963,7 +6197,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>326</v>
       </c>
@@ -5971,7 +6205,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>328</v>
       </c>
@@ -6050,10 +6284,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -6062,7 +6296,7 @@
     <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6070,15 +6304,27 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1157</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>1330</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>346</v>
       </c>
       <c r="B2" t="s">
         <v>347</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1329</v>
       </c>
     </row>
   </sheetData>
@@ -6088,10 +6334,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -6100,7 +6346,7 @@
     <col min="2" max="2" width="18.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6108,10 +6354,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1157</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>1330</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>348</v>
       </c>
@@ -6119,7 +6374,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>350</v>
       </c>
@@ -6127,7 +6382,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>352</v>
       </c>
@@ -6135,7 +6390,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>354</v>
       </c>
@@ -6143,7 +6398,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>356</v>
       </c>
@@ -6151,7 +6406,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>358</v>
       </c>
@@ -6159,7 +6414,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>360</v>
       </c>
@@ -6167,7 +6422,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>362</v>
       </c>
@@ -6175,7 +6430,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>364</v>
       </c>
@@ -6183,7 +6438,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>366</v>
       </c>
@@ -6198,10 +6453,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -6210,7 +6465,7 @@
     <col min="2" max="2" width="28.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6218,10 +6473,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1157</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>1330</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>368</v>
       </c>
@@ -6229,7 +6493,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>370</v>
       </c>
@@ -6237,7 +6501,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>372</v>
       </c>
@@ -6245,7 +6509,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>374</v>
       </c>
@@ -6253,7 +6517,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>376</v>
       </c>
@@ -6261,7 +6525,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>378</v>
       </c>
@@ -6269,7 +6533,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>380</v>
       </c>
@@ -6277,7 +6541,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>382</v>
       </c>
@@ -6285,7 +6549,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>384</v>
       </c>
@@ -6293,7 +6557,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>386</v>
       </c>
@@ -6301,7 +6565,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>388</v>
       </c>
@@ -6309,7 +6573,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>390</v>
       </c>
@@ -6317,7 +6581,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>392</v>
       </c>
@@ -6325,7 +6589,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>394</v>
       </c>
@@ -6333,7 +6597,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>396</v>
       </c>
@@ -6644,10 +6908,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -6656,7 +6920,7 @@
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6664,10 +6928,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1157</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>1330</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>472</v>
       </c>
@@ -6675,7 +6948,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>474</v>
       </c>
@@ -6683,7 +6956,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>476</v>
       </c>
@@ -6691,7 +6964,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>478</v>
       </c>
@@ -6699,7 +6972,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>480</v>
       </c>
@@ -6707,7 +6980,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>482</v>
       </c>
@@ -6715,7 +6988,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>484</v>
       </c>
@@ -6723,7 +6996,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>486</v>
       </c>
@@ -6731,7 +7004,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>488</v>
       </c>
@@ -6739,7 +7012,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>490</v>
       </c>
@@ -6747,7 +7020,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>492</v>
       </c>
@@ -6755,7 +7028,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>494</v>
       </c>
@@ -6763,7 +7036,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>374</v>
       </c>
@@ -6771,7 +7044,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>497</v>
       </c>
@@ -6779,7 +7052,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>499</v>
       </c>
@@ -6978,19 +7251,21 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.3984375" customWidth="1"/>
+    <col min="4" max="4" width="16.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6998,287 +7273,548 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1157</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>1330</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>543</v>
       </c>
       <c r="B2" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1339</v>
+      </c>
+      <c r="E2">
+        <v>300266234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>545</v>
       </c>
       <c r="B3" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>1370</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>547</v>
       </c>
       <c r="B4" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1340</v>
+      </c>
+      <c r="E4">
+        <v>300129361</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>549</v>
       </c>
       <c r="B5" t="s">
         <v>550</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1340</v>
+      </c>
+      <c r="E5">
+        <v>300129361</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>551</v>
       </c>
       <c r="B6" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1341</v>
+      </c>
+      <c r="E6">
+        <v>300127490</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>553</v>
       </c>
       <c r="B7" t="s">
         <v>554</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1342</v>
+      </c>
+      <c r="E7">
+        <v>300311355</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>555</v>
       </c>
       <c r="B8" t="s">
         <v>556</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>557</v>
       </c>
       <c r="B9" t="s">
         <v>558</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1340</v>
+      </c>
+      <c r="E9">
+        <v>300129361</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>559</v>
       </c>
       <c r="B10" t="s">
         <v>560</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1341</v>
+      </c>
+      <c r="E10">
+        <v>300127490</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>561</v>
       </c>
       <c r="B11" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1343</v>
+      </c>
+      <c r="E11">
+        <v>300127794</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>563</v>
       </c>
       <c r="B12" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F12" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>565</v>
       </c>
       <c r="B13" t="s">
         <v>566</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1344</v>
+      </c>
+      <c r="E13">
+        <v>300128438</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>567</v>
       </c>
       <c r="B14" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1345</v>
+      </c>
+      <c r="E14">
+        <v>300266242</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>569</v>
       </c>
       <c r="B15" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1346</v>
+      </c>
+      <c r="E15">
+        <v>300266252</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>571</v>
       </c>
       <c r="B16" t="s">
         <v>572</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="F16" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>573</v>
       </c>
       <c r="B17" t="s">
         <v>574</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1347</v>
+      </c>
+      <c r="E17">
+        <v>300130811</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>575</v>
       </c>
       <c r="B18" t="s">
         <v>576</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1348</v>
+      </c>
+      <c r="E18">
+        <v>300266267</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>577</v>
       </c>
       <c r="B19" t="s">
         <v>578</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1340</v>
+      </c>
+      <c r="E19">
+        <v>300129361</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>579</v>
       </c>
       <c r="B20" t="s">
         <v>580</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1341</v>
+      </c>
+      <c r="E20">
+        <v>300127490</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>581</v>
       </c>
       <c r="B21" t="s">
         <v>582</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="F21" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>583</v>
       </c>
       <c r="B22" t="s">
         <v>584</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="F22" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>585</v>
       </c>
       <c r="B23" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="F23" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>587</v>
       </c>
       <c r="B24" t="s">
         <v>588</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1349</v>
+      </c>
+      <c r="E24">
+        <v>300126734</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>589</v>
       </c>
       <c r="B25" t="s">
         <v>590</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="F25" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>591</v>
       </c>
       <c r="B26" t="s">
         <v>592</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1350</v>
+      </c>
+      <c r="E26">
+        <v>300311191</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>593</v>
       </c>
       <c r="B27" t="s">
         <v>594</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1351</v>
+      </c>
+      <c r="E27">
+        <v>300130257</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>595</v>
       </c>
       <c r="B28" t="s">
         <v>596</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1352</v>
+      </c>
+      <c r="E28">
+        <v>300126225</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>597</v>
       </c>
       <c r="B29" t="s">
         <v>598</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1353</v>
+      </c>
+      <c r="E29">
+        <v>300124707</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>599</v>
       </c>
       <c r="B30" t="s">
         <v>600</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="F30" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>601</v>
       </c>
       <c r="B31" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1354</v>
+      </c>
+      <c r="E31">
+        <v>300266260</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>603</v>
       </c>
       <c r="B32" t="s">
         <v>604</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="F32" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>605</v>
       </c>
       <c r="B33" t="s">
         <v>606</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="F33" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>607</v>
       </c>
       <c r="B34" t="s">
         <v>608</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C34" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1355</v>
+      </c>
+      <c r="E34">
+        <v>300129784</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>609</v>
       </c>
       <c r="B35" t="s">
         <v>610</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D35" t="s">
+        <v>1356</v>
+      </c>
+      <c r="E35">
+        <v>300311368</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>611</v>
       </c>
       <c r="B36" t="s">
         <v>612</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D36" t="s">
+        <v>1357</v>
+      </c>
+      <c r="E36">
+        <v>300130920</v>
       </c>
     </row>
   </sheetData>
@@ -7288,10 +7824,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C140"/>
+  <dimension ref="A1:F140"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -7300,7 +7836,7 @@
     <col min="2" max="2" width="19.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7308,10 +7844,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1157</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>1330</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>613</v>
       </c>
@@ -7319,7 +7864,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>615</v>
       </c>
@@ -7327,7 +7872,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>617</v>
       </c>
@@ -7335,7 +7880,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>619</v>
       </c>
@@ -7343,7 +7888,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>621</v>
       </c>
@@ -7351,7 +7896,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>623</v>
       </c>
@@ -7359,7 +7904,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>625</v>
       </c>
@@ -7367,7 +7912,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>627</v>
       </c>
@@ -7375,7 +7920,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>629</v>
       </c>
@@ -7383,7 +7928,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>631</v>
       </c>
@@ -7391,7 +7936,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>633</v>
       </c>
@@ -7399,7 +7944,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>635</v>
       </c>
@@ -7407,7 +7952,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>637</v>
       </c>
@@ -7415,7 +7960,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>639</v>
       </c>
@@ -7423,7 +7968,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>641</v>
       </c>
@@ -8430,9 +8975,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B162"/>
+  <dimension ref="A1:F162"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -8440,15 +8987,27 @@
     <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="1" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1330</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1158</v>
       </c>
@@ -8456,7 +9015,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1159</v>
       </c>
@@ -8464,7 +9023,7 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1161</v>
       </c>
@@ -8472,7 +9031,7 @@
         <v>1162</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1163</v>
       </c>
@@ -8480,7 +9039,7 @@
         <v>1164</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1165</v>
       </c>
@@ -8488,7 +9047,7 @@
         <v>1166</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1167</v>
       </c>
@@ -8496,7 +9055,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>613</v>
       </c>
@@ -8504,7 +9063,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>615</v>
       </c>
@@ -8512,7 +9071,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>617</v>
       </c>
@@ -8520,7 +9079,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>619</v>
       </c>
@@ -8528,7 +9087,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>621</v>
       </c>
@@ -8536,7 +9095,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>623</v>
       </c>
@@ -8544,7 +9103,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>625</v>
       </c>
@@ -8552,7 +9111,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>627</v>
       </c>
@@ -8560,7 +9119,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>629</v>
       </c>
@@ -9738,15 +10297,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -9755,7 +10315,7 @@
     <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9763,15 +10323,27 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1157</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>1330</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>875</v>
       </c>
       <c r="B2" t="s">
         <v>145</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1329</v>
       </c>
     </row>
   </sheetData>
@@ -9781,10 +10353,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C86"/>
+  <dimension ref="A1:F86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -9793,7 +10365,7 @@
     <col min="2" max="2" width="32.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9801,10 +10373,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1157</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>1330</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>876</v>
       </c>
@@ -9812,7 +10393,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>878</v>
       </c>
@@ -9820,7 +10401,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>880</v>
       </c>
@@ -9828,7 +10409,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>882</v>
       </c>
@@ -9836,7 +10417,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>883</v>
       </c>
@@ -9844,7 +10425,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>885</v>
       </c>
@@ -9852,7 +10433,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>887</v>
       </c>
@@ -9860,7 +10441,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>888</v>
       </c>
@@ -9868,7 +10449,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>890</v>
       </c>
@@ -9876,7 +10457,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>892</v>
       </c>
@@ -9884,7 +10465,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>894</v>
       </c>
@@ -9892,7 +10473,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>896</v>
       </c>
@@ -9900,7 +10481,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>898</v>
       </c>
@@ -9908,7 +10489,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>899</v>
       </c>
@@ -9916,7 +10497,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>900</v>
       </c>
@@ -10491,10 +11072,10 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10502,7 +11083,7 @@
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10510,10 +11091,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1157</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>1330</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1030</v>
       </c>
@@ -10521,7 +11111,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1032</v>
       </c>
@@ -10529,7 +11119,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1034</v>
       </c>
@@ -10537,7 +11127,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>189</v>
       </c>
@@ -10545,7 +11135,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1036</v>
       </c>
@@ -10553,7 +11143,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1036</v>
       </c>
@@ -10561,7 +11151,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1039</v>
       </c>
@@ -10569,7 +11159,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>733</v>
       </c>
@@ -10577,7 +11167,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>296</v>
       </c>
@@ -10585,7 +11175,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>296</v>
       </c>
@@ -10593,7 +11183,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>743</v>
       </c>
@@ -10601,7 +11191,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>1043</v>
       </c>
@@ -10609,7 +11199,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>1045</v>
       </c>
@@ -10617,7 +11207,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>288</v>
       </c>
@@ -10625,7 +11215,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>288</v>
       </c>
@@ -10680,10 +11270,10 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -10692,7 +11282,7 @@
     <col min="2" max="2" width="9.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10700,10 +11290,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1157</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>1330</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1055</v>
       </c>
@@ -10711,7 +11310,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1057</v>
       </c>
@@ -10719,7 +11318,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1058</v>
       </c>
@@ -10727,7 +11326,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1060</v>
       </c>
@@ -10735,7 +11334,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1061</v>
       </c>
@@ -10750,19 +11349,21 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.296875" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10770,16 +11371,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1157</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1330</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>1328</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1062</v>
       </c>
@@ -10787,13 +11391,16 @@
         <v>1063</v>
       </c>
       <c r="C2" t="s">
-        <v>1336</v>
-      </c>
-      <c r="D2">
+        <v>1371</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1372</v>
+      </c>
+      <c r="E2">
         <v>300388256</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1064</v>
       </c>
@@ -10801,13 +11408,16 @@
         <v>1065</v>
       </c>
       <c r="C3" t="s">
-        <v>1335</v>
-      </c>
-      <c r="D3">
+        <v>1371</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1373</v>
+      </c>
+      <c r="E3">
         <v>300388277</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1066</v>
       </c>
@@ -10815,13 +11425,16 @@
         <v>1067</v>
       </c>
       <c r="C4" t="s">
-        <v>1337</v>
-      </c>
-      <c r="D4">
+        <v>1371</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1374</v>
+      </c>
+      <c r="E4">
         <v>300388306</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1068</v>
       </c>
@@ -10829,13 +11442,16 @@
         <v>1069</v>
       </c>
       <c r="C5" t="s">
-        <v>1338</v>
-      </c>
-      <c r="D5">
+        <v>1371</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1375</v>
+      </c>
+      <c r="E5">
         <v>300388344</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>406</v>
       </c>
@@ -10843,13 +11459,16 @@
         <v>1070</v>
       </c>
       <c r="C6" t="s">
-        <v>1339</v>
-      </c>
-      <c r="D6">
+        <v>1371</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1376</v>
+      </c>
+      <c r="E6">
         <v>300387827</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1071</v>
       </c>
@@ -10857,13 +11476,16 @@
         <v>1070</v>
       </c>
       <c r="C7" t="s">
-        <v>1340</v>
-      </c>
-      <c r="D7">
+        <v>1371</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1377</v>
+      </c>
+      <c r="E7">
         <v>300389734</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1072</v>
       </c>
@@ -10871,13 +11493,16 @@
         <v>1073</v>
       </c>
       <c r="C8" t="s">
-        <v>1341</v>
-      </c>
-      <c r="D8">
+        <v>1371</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1378</v>
+      </c>
+      <c r="E8">
         <v>300388401</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1074</v>
       </c>
@@ -10885,13 +11510,16 @@
         <v>1075</v>
       </c>
       <c r="C9" t="s">
-        <v>1342</v>
-      </c>
-      <c r="D9">
+        <v>1371</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1379</v>
+      </c>
+      <c r="E9">
         <v>300388474</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1076</v>
       </c>
@@ -10899,13 +11527,16 @@
         <v>1077</v>
       </c>
       <c r="C10" t="s">
-        <v>1343</v>
-      </c>
-      <c r="D10">
+        <v>1371</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1380</v>
+      </c>
+      <c r="E10">
         <v>300388693</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1078</v>
       </c>
@@ -10913,13 +11544,16 @@
         <v>1079</v>
       </c>
       <c r="C11" t="s">
-        <v>1344</v>
-      </c>
-      <c r="D11">
+        <v>1371</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1381</v>
+      </c>
+      <c r="E11">
         <v>300443706</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1080</v>
       </c>
@@ -10927,13 +11561,16 @@
         <v>1081</v>
       </c>
       <c r="C12" t="s">
-        <v>1345</v>
-      </c>
-      <c r="D12">
+        <v>1371</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1382</v>
+      </c>
+      <c r="E12">
         <v>300389115</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>1082</v>
       </c>
@@ -10941,13 +11578,16 @@
         <v>1083</v>
       </c>
       <c r="C13" t="s">
-        <v>1346</v>
-      </c>
-      <c r="D13">
+        <v>1371</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E13">
         <v>300389311</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>1084</v>
       </c>
@@ -10955,32 +11595,47 @@
         <v>1085</v>
       </c>
       <c r="C14" t="s">
-        <v>1347</v>
-      </c>
-      <c r="D14">
+        <v>1371</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1384</v>
+      </c>
+      <c r="E14">
         <v>300389336</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>1086</v>
       </c>
       <c r="B15" t="s">
         <v>1087</v>
       </c>
-      <c r="E15" t="s">
-        <v>1329</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>1371</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1390</v>
+      </c>
+      <c r="E15">
+        <v>300388737</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>1088</v>
       </c>
       <c r="B16" t="s">
         <v>1089</v>
       </c>
-      <c r="E16" t="s">
-        <v>1329</v>
+      <c r="C16" t="s">
+        <v>1371</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1372</v>
+      </c>
+      <c r="E16">
+        <v>300388256</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -10990,8 +11645,14 @@
       <c r="B17" t="s">
         <v>1091</v>
       </c>
-      <c r="E17" t="s">
-        <v>1329</v>
+      <c r="C17" t="s">
+        <v>1371</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1391</v>
+      </c>
+      <c r="E17">
+        <v>300389645</v>
       </c>
     </row>
   </sheetData>
@@ -11002,19 +11663,21 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.69921875" customWidth="1"/>
+    <col min="4" max="4" width="15.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11022,27 +11685,30 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1157</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1330</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>1328</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>484</v>
       </c>
       <c r="B2" t="s">
         <v>1092</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1093</v>
       </c>
@@ -11050,13 +11716,16 @@
         <v>1094</v>
       </c>
       <c r="C3" t="s">
-        <v>1331</v>
-      </c>
-      <c r="D3">
+        <v>1389</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1385</v>
+      </c>
+      <c r="E3">
         <v>300417206</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1057</v>
       </c>
@@ -11064,13 +11733,16 @@
         <v>1095</v>
       </c>
       <c r="C4" t="s">
-        <v>1332</v>
-      </c>
-      <c r="D4">
+        <v>1389</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1386</v>
+      </c>
+      <c r="E4">
         <v>300055029</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1060</v>
       </c>
@@ -11078,24 +11750,27 @@
         <v>1096</v>
       </c>
       <c r="C5" t="s">
-        <v>1332</v>
-      </c>
-      <c r="D5">
+        <v>1389</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1386</v>
+      </c>
+      <c r="E5">
         <v>300055029</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1097</v>
       </c>
       <c r="B6" t="s">
         <v>1098</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1099</v>
       </c>
@@ -11103,13 +11778,16 @@
         <v>1100</v>
       </c>
       <c r="C7" t="s">
-        <v>1333</v>
-      </c>
-      <c r="D7">
+        <v>1389</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1387</v>
+      </c>
+      <c r="E7">
         <v>300417198</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1101</v>
       </c>
@@ -11117,9 +11795,12 @@
         <v>1102</v>
       </c>
       <c r="C8" t="s">
-        <v>1334</v>
-      </c>
-      <c r="D8">
+        <v>1389</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1388</v>
+      </c>
+      <c r="E8">
         <v>300417196</v>
       </c>
     </row>
@@ -11131,10 +11812,10 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -11143,7 +11824,7 @@
     <col min="2" max="2" width="16.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11151,23 +11832,26 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1157</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1330</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>1328</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1103</v>
       </c>
       <c r="B2" t="s">
         <v>1104</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>1329</v>
       </c>
     </row>
@@ -11178,19 +11862,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.19921875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.09765625" customWidth="1"/>
+    <col min="4" max="4" width="16.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11198,16 +11884,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1157</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1330</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>1328</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -11215,35 +11904,50 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>1348</v>
-      </c>
-      <c r="D2">
+        <v>1359</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1360</v>
+      </c>
+      <c r="E2">
         <v>300435415</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
-        <v>1329</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>1359</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1363</v>
+      </c>
+      <c r="E3">
+        <v>300435425</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" t="s">
-        <v>1329</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>1361</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1364</v>
+      </c>
+      <c r="E4">
+        <v>300435416</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -11251,46 +11955,64 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>1349</v>
-      </c>
-      <c r="D5">
+        <v>1361</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1365</v>
+      </c>
+      <c r="E5">
         <v>300435416</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="E6" t="s">
-        <v>1329</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>1359</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1366</v>
+      </c>
+      <c r="E6">
+        <v>300435438</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="E7" t="s">
-        <v>1329</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>1359</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1331</v>
+      </c>
+      <c r="E7">
+        <v>300435414</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
       </c>
-      <c r="E8" t="s">
-        <v>1329</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>1362</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -11298,32 +12020,44 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>1348</v>
-      </c>
-      <c r="D9">
+        <v>1359</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1360</v>
+      </c>
+      <c r="E9">
         <v>300435415</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>1361</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1364</v>
+      </c>
+      <c r="E10">
+        <v>300435416</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -11331,35 +12065,50 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>1349</v>
-      </c>
-      <c r="D12">
+        <v>1361</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1365</v>
+      </c>
+      <c r="E12">
         <v>300435416</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>21</v>
       </c>
       <c r="B13" t="s">
         <v>22</v>
       </c>
-      <c r="E13" t="s">
-        <v>1329</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>1359</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1331</v>
+      </c>
+      <c r="E13">
+        <v>300435414</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>23</v>
       </c>
       <c r="B14" t="s">
         <v>24</v>
       </c>
-      <c r="E14" t="s">
-        <v>1329</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>1359</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1331</v>
+      </c>
+      <c r="E14">
+        <v>300435414</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -11367,13 +12116,16 @@
         <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>1348</v>
-      </c>
-      <c r="D15">
+        <v>1359</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1360</v>
+      </c>
+      <c r="E15">
         <v>300435415</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -11381,13 +12133,16 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>1348</v>
-      </c>
-      <c r="D16">
+        <v>1359</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1360</v>
+      </c>
+      <c r="E16">
         <v>300435415</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -11395,24 +12150,27 @@
         <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>1349</v>
-      </c>
-      <c r="D17">
+        <v>1361</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1365</v>
+      </c>
+      <c r="E17">
         <v>300435416</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>29</v>
       </c>
       <c r="B18" t="s">
         <v>30</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -11420,10 +12178,35 @@
         <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>1348</v>
-      </c>
-      <c r="D19">
+        <v>1359</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1360</v>
+      </c>
+      <c r="E19">
         <v>300435415</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>1332</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1359</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1332</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1359</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1368</v>
       </c>
     </row>
   </sheetData>
@@ -11434,10 +12217,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+      <selection activeCell="F2" sqref="F2:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -11446,7 +12229,7 @@
     <col min="2" max="2" width="8.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11454,45 +12237,48 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1157</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1330</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>1328</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>33</v>
       </c>
       <c r="B2" t="s">
         <v>34</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>35</v>
       </c>
       <c r="B3" t="s">
         <v>36</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>37</v>
       </c>
       <c r="B4" t="s">
         <v>38</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>1329</v>
       </c>
     </row>
@@ -11503,10 +12289,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+      <selection activeCell="F2" sqref="F2:F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -11515,7 +12301,7 @@
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11523,408 +12309,411 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1157</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1330</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>1328</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>39</v>
       </c>
       <c r="B2" t="s">
         <v>40</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>41</v>
       </c>
       <c r="B3" t="s">
         <v>42</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>43</v>
       </c>
       <c r="B4" t="s">
         <v>44</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>45</v>
       </c>
       <c r="B5" t="s">
         <v>46</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>47</v>
       </c>
       <c r="B6" t="s">
         <v>48</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>49</v>
       </c>
       <c r="B7" t="s">
         <v>50</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>51</v>
       </c>
       <c r="B8" t="s">
         <v>52</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>53</v>
       </c>
       <c r="B9" t="s">
         <v>54</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>55</v>
       </c>
       <c r="B10" t="s">
         <v>56</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>57</v>
       </c>
       <c r="B11" t="s">
         <v>58</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>59</v>
       </c>
       <c r="B12" t="s">
         <v>60</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>61</v>
       </c>
       <c r="B13" t="s">
         <v>62</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>63</v>
       </c>
       <c r="B14" t="s">
         <v>64</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>65</v>
       </c>
       <c r="B15" t="s">
         <v>66</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>67</v>
       </c>
       <c r="B16" t="s">
         <v>68</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>69</v>
       </c>
       <c r="B17" t="s">
         <v>70</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>71</v>
       </c>
       <c r="B18" t="s">
         <v>72</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>73</v>
       </c>
       <c r="B19" t="s">
         <v>74</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>75</v>
       </c>
       <c r="B20" t="s">
         <v>76</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>77</v>
       </c>
       <c r="B21" t="s">
         <v>78</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>79</v>
       </c>
       <c r="B22" t="s">
         <v>80</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>81</v>
       </c>
       <c r="B23" t="s">
         <v>82</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>83</v>
       </c>
       <c r="B24" t="s">
         <v>84</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>85</v>
       </c>
       <c r="B25" t="s">
         <v>86</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>87</v>
       </c>
       <c r="B26" t="s">
         <v>88</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>89</v>
       </c>
       <c r="B27" t="s">
         <v>90</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>91</v>
       </c>
       <c r="B28" t="s">
         <v>92</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>93</v>
       </c>
       <c r="B29" t="s">
         <v>94</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>95</v>
       </c>
       <c r="B30" t="s">
         <v>96</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>97</v>
       </c>
       <c r="B31" t="s">
         <v>98</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>99</v>
       </c>
       <c r="B32" t="s">
         <v>100</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>101</v>
       </c>
       <c r="B33" t="s">
         <v>102</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>103</v>
       </c>
       <c r="B34" t="s">
         <v>104</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>105</v>
       </c>
       <c r="B35" t="s">
         <v>106</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>107</v>
       </c>
       <c r="B36" t="s">
         <v>108</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>109</v>
       </c>
       <c r="B37" t="s">
         <v>110</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>1329</v>
       </c>
     </row>
@@ -11935,10 +12724,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -11947,7 +12736,7 @@
     <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11955,34 +12744,37 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1157</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1330</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>1328</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>111</v>
       </c>
       <c r="B2" t="s">
         <v>112</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>113</v>
       </c>
       <c r="B3" t="s">
         <v>114</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>1329</v>
       </c>
     </row>
@@ -11993,10 +12785,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -12005,7 +12797,7 @@
     <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12013,45 +12805,48 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1157</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1330</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>1328</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>115</v>
       </c>
       <c r="B2" t="s">
         <v>116</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>117</v>
       </c>
       <c r="B3" t="s">
         <v>118</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>119</v>
       </c>
       <c r="B4" t="s">
         <v>120</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>1329</v>
       </c>
     </row>
@@ -12062,10 +12857,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" activeCellId="1" sqref="E2:E5 E20"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -12074,7 +12869,7 @@
     <col min="2" max="2" width="25.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12082,56 +12877,59 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1157</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1330</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>1328</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>121</v>
       </c>
       <c r="B2" t="s">
         <v>122</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>123</v>
       </c>
       <c r="B3" t="s">
         <v>124</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>125</v>
       </c>
       <c r="B4" t="s">
         <v>126</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>127</v>
       </c>
       <c r="B5" t="s">
         <v>128</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>1329</v>
       </c>
     </row>
@@ -12142,10 +12940,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -12154,7 +12952,7 @@
     <col min="2" max="2" width="16.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12162,55 +12960,82 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1157</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>1330</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>129</v>
       </c>
       <c r="B2" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>131</v>
       </c>
       <c r="B3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>133</v>
       </c>
       <c r="B4" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>135</v>
       </c>
       <c r="B5" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>137</v>
       </c>
       <c r="B6" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>139</v>
       </c>
       <c r="B7" t="s">
         <v>132</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1329</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-added sculpture object types -removed objectkenmerken from thesaurus paths
</commit_message>
<xml_diff>
--- a/admin/rdm/Digipolis_Lookup_RDM_Cleaning.xlsx
+++ b/admin/rdm/Digipolis_Lookup_RDM_Cleaning.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="24" yWindow="456" windowWidth="28404" windowHeight="17040" firstSheet="7" activeTab="9"/>
+    <workbookView xWindow="24" yWindow="456" windowWidth="28404" windowHeight="17040" firstSheet="12" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="CSV &lt;-&gt; RDM" sheetId="25" r:id="rId1"/>
@@ -53,7 +53,7 @@
     <definedName name="externe_relatie_types" localSheetId="12">externe_relatie_types.csv!$A$1:$B$24</definedName>
     <definedName name="formaat_types" localSheetId="13">formaat_types.csv!$A$1:$B$2</definedName>
     <definedName name="fotoformaat_types" localSheetId="14">fotoformaat_types.csv!$A$1:$B$11</definedName>
-    <definedName name="genre_types" localSheetId="15">genre_types.csv!$A$1:$B$53</definedName>
+    <definedName name="genre_types" localSheetId="15">genre_types.csv!$A$1:$C$53</definedName>
     <definedName name="isaar_relatie_types" localSheetId="16">isaar_relatie_types.csv!$A$1:$B$39</definedName>
     <definedName name="kleur_types" localSheetId="17">kleur_types.csv!$A$1:$B$36</definedName>
     <definedName name="materiaal_types" localSheetId="18">materiaal_types.csv!$A$1:$B$140</definedName>
@@ -290,7 +290,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1919" uniqueCount="1393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1951" uniqueCount="1408">
   <si>
     <t>code</t>
   </si>
@@ -4369,18 +4369,9 @@
     <t>thesaurus</t>
   </si>
   <si>
-    <t>Digipolis Thesauri\Objectkenmerken\Annotatie Type\</t>
-  </si>
-  <si>
     <t>remarks</t>
   </si>
   <si>
-    <t>Digipolis Thesauri\Objectkenmerken\Beschrijving Type\</t>
-  </si>
-  <si>
-    <t>Digipolis Thesaurus\Objectkenmerken\Annotatie Type\</t>
-  </si>
-  <si>
     <t>condition/examination description</t>
   </si>
   <si>
@@ -4399,15 +4390,6 @@
     <t>related artwork</t>
   </si>
   <si>
-    <t>Digipolis Thesauri\Objectkenmerken\Datumbepaling Type\</t>
-  </si>
-  <si>
-    <t>Digipolis Thesauri\Objectkenmerken\Kleur Type\</t>
-  </si>
-  <si>
-    <t>Digipolis Thesauri\Objectkenmerken\Taal Type\</t>
-  </si>
-  <si>
     <t>Dutch (language)</t>
   </si>
   <si>
@@ -4459,9 +4441,6 @@
     <t>titles proper</t>
   </si>
   <si>
-    <t>Digipolis Thesauri\Objectkenmerken\Titel Type\</t>
-  </si>
-  <si>
     <t>Low German (language)</t>
   </si>
   <si>
@@ -4469,6 +4448,72 @@
   </si>
   <si>
     <t>unidentified (information indicator)</t>
+  </si>
+  <si>
+    <t>filter</t>
+  </si>
+  <si>
+    <t>assemblage (sculpture technique)</t>
+  </si>
+  <si>
+    <t>bas-relief (sculpture technique)</t>
+  </si>
+  <si>
+    <t>busts (general, figures)</t>
+  </si>
+  <si>
+    <t>death masks</t>
+  </si>
+  <si>
+    <t>half figures</t>
+  </si>
+  <si>
+    <t>installations (visual works)</t>
+  </si>
+  <si>
+    <t>heads (representations)</t>
+  </si>
+  <si>
+    <t>medallions (medals)</t>
+  </si>
+  <si>
+    <t>masks (costume)</t>
+  </si>
+  <si>
+    <t>maquettes (sculptures)</t>
+  </si>
+  <si>
+    <t>plaques (flat objects)</t>
+  </si>
+  <si>
+    <t>full-length figures</t>
+  </si>
+  <si>
+    <t>seated figures</t>
+  </si>
+  <si>
+    <t>Digipolis Thesauri\Object Types\sculpture (visual works)\</t>
+  </si>
+  <si>
+    <t>Digipolis Thesauri\Annotatie Type\</t>
+  </si>
+  <si>
+    <t>Digipolis Thesauri\Beschrijving Type\</t>
+  </si>
+  <si>
+    <t>Digipolis Thesaurus\Annotatie Type\</t>
+  </si>
+  <si>
+    <t>Digipolis Thesauri\Datumbepaling Type\</t>
+  </si>
+  <si>
+    <t>Digipolis Thesauri\Kleur Type\</t>
+  </si>
+  <si>
+    <t>Digipolis Thesauri\Taal Type\</t>
+  </si>
+  <si>
+    <t>Digipolis Thesauri\Titel Type\</t>
   </si>
 </sst>
 </file>
@@ -5171,8 +5216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -5222,7 +5267,7 @@
         <v>143</v>
       </c>
       <c r="C3" t="s">
-        <v>1369</v>
+        <v>1404</v>
       </c>
       <c r="D3" t="s">
         <v>1334</v>
@@ -5239,7 +5284,7 @@
         <v>145</v>
       </c>
       <c r="C4" t="s">
-        <v>1369</v>
+        <v>1404</v>
       </c>
       <c r="D4" t="s">
         <v>1334</v>
@@ -5256,7 +5301,7 @@
         <v>147</v>
       </c>
       <c r="C5" t="s">
-        <v>1369</v>
+        <v>1404</v>
       </c>
       <c r="D5" t="s">
         <v>1335</v>
@@ -5273,7 +5318,7 @@
         <v>149</v>
       </c>
       <c r="C6" t="s">
-        <v>1369</v>
+        <v>1404</v>
       </c>
       <c r="D6" t="s">
         <v>1336</v>
@@ -5287,10 +5332,10 @@
         <v>151</v>
       </c>
       <c r="C7" t="s">
-        <v>1369</v>
+        <v>1404</v>
       </c>
       <c r="D7" t="s">
-        <v>1392</v>
+        <v>1385</v>
       </c>
       <c r="E7">
         <v>300386154</v>
@@ -5304,7 +5349,7 @@
         <v>153</v>
       </c>
       <c r="C8" t="s">
-        <v>1369</v>
+        <v>1404</v>
       </c>
       <c r="D8" t="s">
         <v>1337</v>
@@ -5318,7 +5363,7 @@
         <v>155</v>
       </c>
       <c r="C9" t="s">
-        <v>1369</v>
+        <v>1404</v>
       </c>
       <c r="D9" t="s">
         <v>1338</v>
@@ -5332,7 +5377,7 @@
         <v>157</v>
       </c>
       <c r="C10" t="s">
-        <v>1369</v>
+        <v>1404</v>
       </c>
       <c r="D10" t="s">
         <v>1334</v>
@@ -6453,451 +6498,593 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.19921875" customWidth="1"/>
+    <col min="3" max="3" width="28.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1386</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1358</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1157</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>1330</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>1328</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>368</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>370</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>372</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>374</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>376</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>378</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>1400</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1387</v>
+      </c>
+      <c r="F7">
+        <v>300138696</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>380</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>1400</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1387</v>
+      </c>
+      <c r="F8">
+        <v>300138696</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>382</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>1400</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1388</v>
+      </c>
+      <c r="F9">
+        <v>300053623</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>384</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>1400</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1389</v>
+      </c>
+      <c r="F10">
+        <v>300047457</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>386</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>1400</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1390</v>
+      </c>
+      <c r="F11">
+        <v>300047724</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>388</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>1400</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F12">
+        <v>300047469</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>390</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>392</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>1400</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1390</v>
+      </c>
+      <c r="F14">
+        <v>300047724</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>394</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>1400</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1392</v>
+      </c>
+      <c r="F15">
+        <v>300047896</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>396</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>1400</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1393</v>
+      </c>
+      <c r="F16">
+        <v>300262520</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>398</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>1400</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1394</v>
+      </c>
+      <c r="F17">
+        <v>300077357</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>400</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>1400</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1395</v>
+      </c>
+      <c r="F18">
+        <v>300138758</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>402</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>1400</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1396</v>
+      </c>
+      <c r="F19">
+        <v>300047837</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>404</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
+        <v>1400</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1397</v>
+      </c>
+      <c r="F20">
+        <v>300010262</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>406</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="G21" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>408</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D22" t="s">
+        <v>1400</v>
+      </c>
+      <c r="E22" t="s">
+        <v>1398</v>
+      </c>
+      <c r="F22">
+        <v>300343592</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>410</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>1400</v>
+      </c>
+      <c r="E23" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F23">
+        <v>300404835</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>412</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>414</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>416</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>418</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>420</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>422</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>424</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>426</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>428</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>430</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>432</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>434</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>436</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>438</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>440</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>442</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>444</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>446</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>448</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>450</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>452</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>454</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>456</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>458</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>460</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>462</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>464</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C50" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>466</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>468</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>470</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" t="s">
         <v>471</v>
       </c>
     </row>
@@ -7293,7 +7480,7 @@
         <v>544</v>
       </c>
       <c r="C2" t="s">
-        <v>1370</v>
+        <v>1405</v>
       </c>
       <c r="D2" t="s">
         <v>1339</v>
@@ -7310,7 +7497,7 @@
         <v>546</v>
       </c>
       <c r="C3" t="s">
-        <v>1370</v>
+        <v>1405</v>
       </c>
       <c r="F3" t="s">
         <v>1329</v>
@@ -7324,7 +7511,7 @@
         <v>548</v>
       </c>
       <c r="C4" t="s">
-        <v>1370</v>
+        <v>1405</v>
       </c>
       <c r="D4" t="s">
         <v>1340</v>
@@ -7341,7 +7528,7 @@
         <v>550</v>
       </c>
       <c r="C5" t="s">
-        <v>1370</v>
+        <v>1405</v>
       </c>
       <c r="D5" t="s">
         <v>1340</v>
@@ -7358,7 +7545,7 @@
         <v>552</v>
       </c>
       <c r="C6" t="s">
-        <v>1370</v>
+        <v>1405</v>
       </c>
       <c r="D6" t="s">
         <v>1341</v>
@@ -7375,7 +7562,7 @@
         <v>554</v>
       </c>
       <c r="C7" t="s">
-        <v>1370</v>
+        <v>1405</v>
       </c>
       <c r="D7" t="s">
         <v>1342</v>
@@ -7403,7 +7590,7 @@
         <v>558</v>
       </c>
       <c r="C9" t="s">
-        <v>1370</v>
+        <v>1405</v>
       </c>
       <c r="D9" t="s">
         <v>1340</v>
@@ -7420,7 +7607,7 @@
         <v>560</v>
       </c>
       <c r="C10" t="s">
-        <v>1370</v>
+        <v>1405</v>
       </c>
       <c r="D10" t="s">
         <v>1341</v>
@@ -7437,7 +7624,7 @@
         <v>562</v>
       </c>
       <c r="C11" t="s">
-        <v>1370</v>
+        <v>1405</v>
       </c>
       <c r="D11" t="s">
         <v>1343</v>
@@ -7465,7 +7652,7 @@
         <v>566</v>
       </c>
       <c r="C13" t="s">
-        <v>1370</v>
+        <v>1405</v>
       </c>
       <c r="D13" t="s">
         <v>1344</v>
@@ -7482,7 +7669,7 @@
         <v>568</v>
       </c>
       <c r="C14" t="s">
-        <v>1370</v>
+        <v>1405</v>
       </c>
       <c r="D14" t="s">
         <v>1345</v>
@@ -7499,7 +7686,7 @@
         <v>570</v>
       </c>
       <c r="C15" t="s">
-        <v>1370</v>
+        <v>1405</v>
       </c>
       <c r="D15" t="s">
         <v>1346</v>
@@ -7527,7 +7714,7 @@
         <v>574</v>
       </c>
       <c r="C17" t="s">
-        <v>1370</v>
+        <v>1405</v>
       </c>
       <c r="D17" t="s">
         <v>1347</v>
@@ -7544,7 +7731,7 @@
         <v>576</v>
       </c>
       <c r="C18" t="s">
-        <v>1370</v>
+        <v>1405</v>
       </c>
       <c r="D18" t="s">
         <v>1348</v>
@@ -7561,7 +7748,7 @@
         <v>578</v>
       </c>
       <c r="C19" t="s">
-        <v>1370</v>
+        <v>1405</v>
       </c>
       <c r="D19" t="s">
         <v>1340</v>
@@ -7578,7 +7765,7 @@
         <v>580</v>
       </c>
       <c r="C20" t="s">
-        <v>1370</v>
+        <v>1405</v>
       </c>
       <c r="D20" t="s">
         <v>1341</v>
@@ -7628,7 +7815,7 @@
         <v>588</v>
       </c>
       <c r="C24" t="s">
-        <v>1370</v>
+        <v>1405</v>
       </c>
       <c r="D24" t="s">
         <v>1349</v>
@@ -7656,7 +7843,7 @@
         <v>592</v>
       </c>
       <c r="C26" t="s">
-        <v>1370</v>
+        <v>1405</v>
       </c>
       <c r="D26" t="s">
         <v>1350</v>
@@ -7673,7 +7860,7 @@
         <v>594</v>
       </c>
       <c r="C27" t="s">
-        <v>1370</v>
+        <v>1405</v>
       </c>
       <c r="D27" t="s">
         <v>1351</v>
@@ -7690,7 +7877,7 @@
         <v>596</v>
       </c>
       <c r="C28" t="s">
-        <v>1370</v>
+        <v>1405</v>
       </c>
       <c r="D28" t="s">
         <v>1352</v>
@@ -7707,7 +7894,7 @@
         <v>598</v>
       </c>
       <c r="C29" t="s">
-        <v>1370</v>
+        <v>1405</v>
       </c>
       <c r="D29" t="s">
         <v>1353</v>
@@ -7735,7 +7922,7 @@
         <v>602</v>
       </c>
       <c r="C31" t="s">
-        <v>1370</v>
+        <v>1405</v>
       </c>
       <c r="D31" t="s">
         <v>1354</v>
@@ -7774,7 +7961,7 @@
         <v>608</v>
       </c>
       <c r="C34" t="s">
-        <v>1370</v>
+        <v>1405</v>
       </c>
       <c r="D34" t="s">
         <v>1355</v>
@@ -7791,7 +7978,7 @@
         <v>610</v>
       </c>
       <c r="C35" t="s">
-        <v>1370</v>
+        <v>1405</v>
       </c>
       <c r="D35" t="s">
         <v>1356</v>
@@ -7808,7 +7995,7 @@
         <v>612</v>
       </c>
       <c r="C36" t="s">
-        <v>1370</v>
+        <v>1405</v>
       </c>
       <c r="D36" t="s">
         <v>1357</v>
@@ -11391,10 +11578,10 @@
         <v>1063</v>
       </c>
       <c r="C2" t="s">
-        <v>1371</v>
+        <v>1406</v>
       </c>
       <c r="D2" t="s">
-        <v>1372</v>
+        <v>1366</v>
       </c>
       <c r="E2">
         <v>300388256</v>
@@ -11408,10 +11595,10 @@
         <v>1065</v>
       </c>
       <c r="C3" t="s">
-        <v>1371</v>
+        <v>1406</v>
       </c>
       <c r="D3" t="s">
-        <v>1373</v>
+        <v>1367</v>
       </c>
       <c r="E3">
         <v>300388277</v>
@@ -11425,10 +11612,10 @@
         <v>1067</v>
       </c>
       <c r="C4" t="s">
-        <v>1371</v>
+        <v>1406</v>
       </c>
       <c r="D4" t="s">
-        <v>1374</v>
+        <v>1368</v>
       </c>
       <c r="E4">
         <v>300388306</v>
@@ -11442,10 +11629,10 @@
         <v>1069</v>
       </c>
       <c r="C5" t="s">
-        <v>1371</v>
+        <v>1406</v>
       </c>
       <c r="D5" t="s">
-        <v>1375</v>
+        <v>1369</v>
       </c>
       <c r="E5">
         <v>300388344</v>
@@ -11459,10 +11646,10 @@
         <v>1070</v>
       </c>
       <c r="C6" t="s">
-        <v>1371</v>
+        <v>1406</v>
       </c>
       <c r="D6" t="s">
-        <v>1376</v>
+        <v>1370</v>
       </c>
       <c r="E6">
         <v>300387827</v>
@@ -11476,10 +11663,10 @@
         <v>1070</v>
       </c>
       <c r="C7" t="s">
+        <v>1406</v>
+      </c>
+      <c r="D7" t="s">
         <v>1371</v>
-      </c>
-      <c r="D7" t="s">
-        <v>1377</v>
       </c>
       <c r="E7">
         <v>300389734</v>
@@ -11493,10 +11680,10 @@
         <v>1073</v>
       </c>
       <c r="C8" t="s">
-        <v>1371</v>
+        <v>1406</v>
       </c>
       <c r="D8" t="s">
-        <v>1378</v>
+        <v>1372</v>
       </c>
       <c r="E8">
         <v>300388401</v>
@@ -11510,10 +11697,10 @@
         <v>1075</v>
       </c>
       <c r="C9" t="s">
-        <v>1371</v>
+        <v>1406</v>
       </c>
       <c r="D9" t="s">
-        <v>1379</v>
+        <v>1373</v>
       </c>
       <c r="E9">
         <v>300388474</v>
@@ -11527,10 +11714,10 @@
         <v>1077</v>
       </c>
       <c r="C10" t="s">
-        <v>1371</v>
+        <v>1406</v>
       </c>
       <c r="D10" t="s">
-        <v>1380</v>
+        <v>1374</v>
       </c>
       <c r="E10">
         <v>300388693</v>
@@ -11544,10 +11731,10 @@
         <v>1079</v>
       </c>
       <c r="C11" t="s">
-        <v>1371</v>
+        <v>1406</v>
       </c>
       <c r="D11" t="s">
-        <v>1381</v>
+        <v>1375</v>
       </c>
       <c r="E11">
         <v>300443706</v>
@@ -11561,10 +11748,10 @@
         <v>1081</v>
       </c>
       <c r="C12" t="s">
-        <v>1371</v>
+        <v>1406</v>
       </c>
       <c r="D12" t="s">
-        <v>1382</v>
+        <v>1376</v>
       </c>
       <c r="E12">
         <v>300389115</v>
@@ -11578,10 +11765,10 @@
         <v>1083</v>
       </c>
       <c r="C13" t="s">
-        <v>1371</v>
+        <v>1406</v>
       </c>
       <c r="D13" t="s">
-        <v>1383</v>
+        <v>1377</v>
       </c>
       <c r="E13">
         <v>300389311</v>
@@ -11595,10 +11782,10 @@
         <v>1085</v>
       </c>
       <c r="C14" t="s">
-        <v>1371</v>
+        <v>1406</v>
       </c>
       <c r="D14" t="s">
-        <v>1384</v>
+        <v>1378</v>
       </c>
       <c r="E14">
         <v>300389336</v>
@@ -11612,10 +11799,10 @@
         <v>1087</v>
       </c>
       <c r="C15" t="s">
-        <v>1371</v>
+        <v>1406</v>
       </c>
       <c r="D15" t="s">
-        <v>1390</v>
+        <v>1383</v>
       </c>
       <c r="E15">
         <v>300388737</v>
@@ -11629,10 +11816,10 @@
         <v>1089</v>
       </c>
       <c r="C16" t="s">
-        <v>1371</v>
+        <v>1406</v>
       </c>
       <c r="D16" t="s">
-        <v>1372</v>
+        <v>1366</v>
       </c>
       <c r="E16">
         <v>300388256</v>
@@ -11646,10 +11833,10 @@
         <v>1091</v>
       </c>
       <c r="C17" t="s">
-        <v>1371</v>
+        <v>1406</v>
       </c>
       <c r="D17" t="s">
-        <v>1391</v>
+        <v>1384</v>
       </c>
       <c r="E17">
         <v>300389645</v>
@@ -11716,10 +11903,10 @@
         <v>1094</v>
       </c>
       <c r="C3" t="s">
-        <v>1389</v>
+        <v>1407</v>
       </c>
       <c r="D3" t="s">
-        <v>1385</v>
+        <v>1379</v>
       </c>
       <c r="E3">
         <v>300417206</v>
@@ -11733,10 +11920,10 @@
         <v>1095</v>
       </c>
       <c r="C4" t="s">
-        <v>1389</v>
+        <v>1407</v>
       </c>
       <c r="D4" t="s">
-        <v>1386</v>
+        <v>1380</v>
       </c>
       <c r="E4">
         <v>300055029</v>
@@ -11750,10 +11937,10 @@
         <v>1096</v>
       </c>
       <c r="C5" t="s">
-        <v>1389</v>
+        <v>1407</v>
       </c>
       <c r="D5" t="s">
-        <v>1386</v>
+        <v>1380</v>
       </c>
       <c r="E5">
         <v>300055029</v>
@@ -11778,10 +11965,10 @@
         <v>1100</v>
       </c>
       <c r="C7" t="s">
-        <v>1389</v>
+        <v>1407</v>
       </c>
       <c r="D7" t="s">
-        <v>1387</v>
+        <v>1381</v>
       </c>
       <c r="E7">
         <v>300417198</v>
@@ -11795,10 +11982,10 @@
         <v>1102</v>
       </c>
       <c r="C8" t="s">
-        <v>1389</v>
+        <v>1407</v>
       </c>
       <c r="D8" t="s">
-        <v>1388</v>
+        <v>1382</v>
       </c>
       <c r="E8">
         <v>300417196</v>
@@ -11904,10 +12091,10 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
+        <v>1401</v>
+      </c>
+      <c r="D2" t="s">
         <v>1359</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1360</v>
       </c>
       <c r="E2">
         <v>300435415</v>
@@ -11921,10 +12108,10 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>1359</v>
+        <v>1401</v>
       </c>
       <c r="D3" t="s">
-        <v>1363</v>
+        <v>1360</v>
       </c>
       <c r="E3">
         <v>300435425</v>
@@ -11938,10 +12125,10 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
+        <v>1402</v>
+      </c>
+      <c r="D4" t="s">
         <v>1361</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1364</v>
       </c>
       <c r="E4">
         <v>300435416</v>
@@ -11955,10 +12142,10 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>1361</v>
+        <v>1402</v>
       </c>
       <c r="D5" t="s">
-        <v>1365</v>
+        <v>1362</v>
       </c>
       <c r="E5">
         <v>300435416</v>
@@ -11972,10 +12159,10 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>1359</v>
+        <v>1401</v>
       </c>
       <c r="D6" t="s">
-        <v>1366</v>
+        <v>1363</v>
       </c>
       <c r="E6">
         <v>300435438</v>
@@ -11989,7 +12176,7 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>1359</v>
+        <v>1401</v>
       </c>
       <c r="D7" t="s">
         <v>1331</v>
@@ -12006,10 +12193,10 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>1362</v>
+        <v>1403</v>
       </c>
       <c r="D8" t="s">
-        <v>1367</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -12020,10 +12207,10 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
+        <v>1401</v>
+      </c>
+      <c r="D9" t="s">
         <v>1359</v>
-      </c>
-      <c r="D9" t="s">
-        <v>1360</v>
       </c>
       <c r="E9">
         <v>300435415</v>
@@ -12037,10 +12224,10 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
+        <v>1402</v>
+      </c>
+      <c r="D10" t="s">
         <v>1361</v>
-      </c>
-      <c r="D10" t="s">
-        <v>1364</v>
       </c>
       <c r="E10">
         <v>300435416</v>
@@ -12065,10 +12252,10 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>1361</v>
+        <v>1402</v>
       </c>
       <c r="D12" t="s">
-        <v>1365</v>
+        <v>1362</v>
       </c>
       <c r="E12">
         <v>300435416</v>
@@ -12082,7 +12269,7 @@
         <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>1359</v>
+        <v>1401</v>
       </c>
       <c r="D13" t="s">
         <v>1331</v>
@@ -12099,7 +12286,7 @@
         <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>1359</v>
+        <v>1401</v>
       </c>
       <c r="D14" t="s">
         <v>1331</v>
@@ -12116,10 +12303,10 @@
         <v>26</v>
       </c>
       <c r="C15" t="s">
+        <v>1401</v>
+      </c>
+      <c r="D15" t="s">
         <v>1359</v>
-      </c>
-      <c r="D15" t="s">
-        <v>1360</v>
       </c>
       <c r="E15">
         <v>300435415</v>
@@ -12133,10 +12320,10 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
+        <v>1401</v>
+      </c>
+      <c r="D16" t="s">
         <v>1359</v>
-      </c>
-      <c r="D16" t="s">
-        <v>1360</v>
       </c>
       <c r="E16">
         <v>300435415</v>
@@ -12150,10 +12337,10 @@
         <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>1361</v>
+        <v>1402</v>
       </c>
       <c r="D17" t="s">
-        <v>1365</v>
+        <v>1362</v>
       </c>
       <c r="E17">
         <v>300435416</v>
@@ -12178,10 +12365,10 @@
         <v>26</v>
       </c>
       <c r="C19" t="s">
+        <v>1401</v>
+      </c>
+      <c r="D19" t="s">
         <v>1359</v>
-      </c>
-      <c r="D19" t="s">
-        <v>1360</v>
       </c>
       <c r="E19">
         <v>300435415</v>
@@ -12192,7 +12379,7 @@
         <v>1332</v>
       </c>
       <c r="C20" t="s">
-        <v>1359</v>
+        <v>1401</v>
       </c>
       <c r="D20" t="s">
         <v>1332</v>
@@ -12203,10 +12390,10 @@
         <v>1333</v>
       </c>
       <c r="C21" t="s">
-        <v>1359</v>
+        <v>1401</v>
       </c>
       <c r="D21" t="s">
-        <v>1368</v>
+        <v>1365</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
double checked possibly ambiguous material and carrier values
</commit_message>
<xml_diff>
--- a/admin/rdm/Digipolis_Lookup_RDM_Cleaning.xlsx
+++ b/admin/rdm/Digipolis_Lookup_RDM_Cleaning.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="24" yWindow="456" windowWidth="28404" windowHeight="17040" activeTab="20"/>
+    <workbookView xWindow="24" yWindow="456" windowWidth="28404" windowHeight="17040" firstSheet="14" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="CSV &lt;-&gt; RDM" sheetId="25" r:id="rId1"/>
@@ -40,7 +40,7 @@
     <sheet name="toegang_types.csv" sheetId="24" r:id="rId26"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">materiaal_types.csv!$A$1:$F$142</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">materiaal_types.csv!$A$1:$F$145</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">techniek_types.csv!$A$1:$F$162</definedName>
     <definedName name="annotatie_types" localSheetId="2">annotatie_types.csv!$A$1:$B$19</definedName>
     <definedName name="av_film_materiaal_types" localSheetId="3">av_film_materiaal_types.csv!$A$1:$B$4</definedName>
@@ -58,7 +58,7 @@
     <definedName name="genre_types" localSheetId="15">genre_types.csv!$A$1:$C$53</definedName>
     <definedName name="isaar_relatie_types" localSheetId="16">isaar_relatie_types.csv!$A$1:$B$39</definedName>
     <definedName name="kleur_types" localSheetId="17">kleur_types.csv!$A$1:$B$36</definedName>
-    <definedName name="materiaal_types" localSheetId="18">materiaal_types.csv!$A$1:$B$142</definedName>
+    <definedName name="materiaal_types" localSheetId="18">materiaal_types.csv!$A$1:$B$145</definedName>
     <definedName name="numberofpages_qualifier_types" localSheetId="19">numberofpages_qualifier_types.c!$A$1:$B$2</definedName>
     <definedName name="object_types" localSheetId="20">object_types.csv!$A$1:$B$86</definedName>
     <definedName name="record_types" localSheetId="21">'record_types.csv'!$A$1:$B$21</definedName>
@@ -292,7 +292,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2531" uniqueCount="1587">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2549" uniqueCount="1591">
   <si>
     <t>code</t>
   </si>
@@ -5056,6 +5056,24 @@
   </si>
   <si>
     <t>pencils</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kenmerken/lhmateriaalaanvob/lhmateriaalsoortob
+</t>
+  </si>
+  <si>
+    <t>kenmerken/lhdragerico/lhdragertypeico
+kenmerken/lhdragerps
+kenmerken/mpmdragerak
+kenmerken/mpmdragertk</t>
+  </si>
+  <si>
+    <t>kenmerken/lhdragerico/lhdragertypeico
+kenmerken/lhdragerps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kenmerken/lhmateriaalob/lhmateriaalsoortob
+</t>
   </si>
 </sst>
 </file>
@@ -7213,8 +7231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -9034,18 +9052,22 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:G142"/>
+  <dimension ref="A1:G145"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A128" sqref="A128"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.5" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.296875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="11.19921875" style="6"/>
+    <col min="3" max="3" width="34.19921875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="18.5" style="6" customWidth="1"/>
+    <col min="5" max="6" width="11.19921875" style="6"/>
+    <col min="7" max="7" width="49.19921875" style="6" customWidth="1"/>
+    <col min="8" max="16384" width="11.19921875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -10214,8 +10236,8 @@
         <v>300014109</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A75" s="6" t="s">
+    <row r="75" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A75" s="13" t="s">
         <v>748</v>
       </c>
       <c r="B75" s="6" t="s">
@@ -10230,242 +10252,248 @@
       <c r="E75" s="8">
         <v>300014224</v>
       </c>
+      <c r="G75" s="12" t="s">
+        <v>1589</v>
+      </c>
     </row>
     <row r="76" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A76" s="6" t="s">
-        <v>750</v>
+      <c r="A76" s="13" t="s">
+        <v>748</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>654</v>
+        <v>749</v>
       </c>
       <c r="C76" s="6" t="s">
         <v>1564</v>
       </c>
       <c r="D76" s="7" t="s">
+        <v>1574</v>
+      </c>
+      <c r="E76" s="8">
+        <v>300014224</v>
+      </c>
+      <c r="G76" s="12" t="s">
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A77" s="6" t="s">
+        <v>750</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>1564</v>
+      </c>
+      <c r="D77" s="7" t="s">
         <v>1540</v>
       </c>
-      <c r="E76" s="8">
+      <c r="E77" s="8">
         <v>300014570</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A77" s="6" t="s">
+    <row r="78" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A78" s="6" t="s">
         <v>751</v>
       </c>
-      <c r="B77" s="6" t="s">
+      <c r="B78" s="6" t="s">
         <v>752</v>
       </c>
-      <c r="C77" s="6" t="s">
+      <c r="C78" s="6" t="s">
         <v>1569</v>
       </c>
-      <c r="D77" s="7" t="s">
+      <c r="D78" s="7" t="s">
         <v>1568</v>
       </c>
-      <c r="E77" s="8">
+      <c r="E78" s="8">
         <v>300014069</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A78" s="6" t="s">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A79" s="6" t="s">
         <v>753</v>
       </c>
-      <c r="B78" s="6" t="s">
+      <c r="B79" s="6" t="s">
         <v>754</v>
       </c>
-      <c r="C78" s="6" t="s">
+      <c r="C79" s="6" t="s">
         <v>1564</v>
       </c>
-      <c r="D78" s="7" t="s">
+      <c r="D79" s="7" t="s">
         <v>1541</v>
       </c>
-      <c r="E78" s="8">
+      <c r="E79" s="8">
         <v>300011845</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A79" s="6" t="s">
+    <row r="80" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A80" s="6" t="s">
         <v>755</v>
       </c>
-      <c r="B79" s="6" t="s">
+      <c r="B80" s="6" t="s">
         <v>756</v>
       </c>
-      <c r="C79" s="6" t="s">
+      <c r="C80" s="6" t="s">
         <v>1569</v>
       </c>
-      <c r="D79" s="7" t="s">
+      <c r="D80" s="7" t="s">
         <v>1568</v>
       </c>
-      <c r="E79" s="8">
+      <c r="E80" s="8">
         <v>300014069</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A80" s="6" t="s">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A81" s="6" t="s">
         <v>757</v>
       </c>
-      <c r="B80" s="6" t="s">
+      <c r="B81" s="6" t="s">
         <v>758</v>
       </c>
-      <c r="C80" s="6" t="s">
+      <c r="C81" s="6" t="s">
         <v>1564</v>
       </c>
-      <c r="D80" s="7" t="s">
+      <c r="D81" s="7" t="s">
         <v>1542</v>
       </c>
-      <c r="E80" s="8">
+      <c r="E81" s="8">
         <v>300011022</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A81" s="6" t="s">
+    <row r="82" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A82" s="6" t="s">
         <v>759</v>
       </c>
-      <c r="B81" s="6" t="s">
+      <c r="B82" s="6" t="s">
         <v>760</v>
       </c>
-      <c r="C81" s="6" t="s">
+      <c r="C82" s="6" t="s">
         <v>1569</v>
       </c>
-      <c r="D81" s="7" t="s">
+      <c r="D82" s="7" t="s">
         <v>1567</v>
       </c>
-      <c r="E81" s="8">
+      <c r="E82" s="8">
         <v>300014109</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A82" s="6" t="s">
+    <row r="83" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A83" s="6" t="s">
         <v>761</v>
       </c>
-      <c r="B82" s="6" t="s">
+      <c r="B83" s="6" t="s">
         <v>660</v>
       </c>
-      <c r="C82" s="6" t="s">
+      <c r="C83" s="6" t="s">
         <v>1564</v>
       </c>
-      <c r="D82" s="7" t="s">
+      <c r="D83" s="7" t="s">
         <v>1543</v>
       </c>
-      <c r="E82" s="8">
+      <c r="E83" s="8">
         <v>300011443</v>
       </c>
-      <c r="F82" s="11" t="s">
+      <c r="F83" s="11" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A83" s="6" t="s">
+    <row r="84" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A84" s="6" t="s">
         <v>762</v>
       </c>
-      <c r="B83" s="6" t="s">
+      <c r="B84" s="6" t="s">
         <v>763</v>
       </c>
-      <c r="C83" s="6" t="s">
+      <c r="C84" s="6" t="s">
         <v>1569</v>
       </c>
-      <c r="D83" s="7" t="s">
+      <c r="D84" s="7" t="s">
         <v>1576</v>
       </c>
-      <c r="E83" s="8">
+      <c r="E84" s="8">
         <v>300390932</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A84" s="6" t="s">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A85" s="6" t="s">
         <v>764</v>
       </c>
-      <c r="B84" s="6" t="s">
+      <c r="B85" s="6" t="s">
         <v>765</v>
       </c>
-      <c r="C84" s="6" t="s">
+      <c r="C85" s="6" t="s">
         <v>1564</v>
       </c>
-      <c r="D84" s="7" t="s">
+      <c r="D85" s="7" t="s">
         <v>1544</v>
       </c>
-      <c r="E84" s="8">
+      <c r="E85" s="8">
         <v>300010900</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A85" s="6" t="s">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A86" s="6" t="s">
         <v>766</v>
       </c>
-      <c r="B85" s="6" t="s">
+      <c r="B86" s="6" t="s">
         <v>767</v>
-      </c>
-      <c r="F85" s="6" t="s">
-        <v>1329</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A86" s="6" t="s">
-        <v>768</v>
-      </c>
-      <c r="B86" s="6" t="s">
-        <v>327</v>
       </c>
       <c r="F86" s="6" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="6" t="s">
+        <v>768</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="F87" s="6" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A88" s="6" t="s">
         <v>769</v>
       </c>
-      <c r="B87" s="6" t="s">
+      <c r="B88" s="6" t="s">
         <v>770</v>
-      </c>
-      <c r="C87" s="6" t="s">
-        <v>1569</v>
-      </c>
-      <c r="D87" s="7" t="s">
-        <v>1577</v>
-      </c>
-      <c r="E87" s="8">
-        <v>300014657</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A88" s="6" t="s">
-        <v>771</v>
-      </c>
-      <c r="B88" s="6" t="s">
-        <v>772</v>
       </c>
       <c r="C88" s="6" t="s">
         <v>1569</v>
       </c>
       <c r="D88" s="7" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="E88" s="8">
-        <v>300011851</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+        <v>300014657</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A89" s="6" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="C89" s="6" t="s">
         <v>1569</v>
       </c>
       <c r="D89" s="7" t="s">
-        <v>1567</v>
+        <v>1578</v>
       </c>
       <c r="E89" s="8">
-        <v>300014109</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+        <v>300011851</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A90" s="6" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="C90" s="6" t="s">
         <v>1569</v>
@@ -10477,63 +10505,63 @@
         <v>300014109</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A91" s="6" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="C91" s="6" t="s">
         <v>1569</v>
       </c>
       <c r="D91" s="7" t="s">
+        <v>1567</v>
+      </c>
+      <c r="E91" s="8">
+        <v>300014109</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A92" s="6" t="s">
+        <v>777</v>
+      </c>
+      <c r="B92" s="6" t="s">
+        <v>778</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>1569</v>
+      </c>
+      <c r="D92" s="7" t="s">
         <v>1578</v>
       </c>
-      <c r="E91" s="8">
+      <c r="E92" s="8">
         <v>300011851</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A92" s="6" t="s">
+    <row r="93" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A93" s="6" t="s">
         <v>779</v>
       </c>
-      <c r="B92" s="6" t="s">
+      <c r="B93" s="6" t="s">
         <v>780</v>
       </c>
-      <c r="C92" s="6" t="s">
+      <c r="C93" s="6" t="s">
         <v>1564</v>
       </c>
-      <c r="D92" s="7" t="s">
+      <c r="D93" s="7" t="s">
         <v>1554</v>
       </c>
-      <c r="E92" s="8">
+      <c r="E93" s="8">
         <v>300010662</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A93" s="6" t="s">
+    <row r="94" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A94" s="13" t="s">
         <v>781</v>
       </c>
-      <c r="B93" s="6" t="s">
+      <c r="B94" s="6" t="s">
         <v>782</v>
-      </c>
-      <c r="C93" s="6" t="s">
-        <v>1569</v>
-      </c>
-      <c r="D93" s="7" t="s">
-        <v>1567</v>
-      </c>
-      <c r="E93" s="8">
-        <v>300014109</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A94" s="6" t="s">
-        <v>783</v>
-      </c>
-      <c r="B94" s="6" t="s">
-        <v>784</v>
       </c>
       <c r="C94" s="6" t="s">
         <v>1569</v>
@@ -10544,16 +10572,19 @@
       <c r="E94" s="8">
         <v>300014109</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A95" s="6" t="s">
-        <v>785</v>
+      <c r="G94" s="12" t="s">
+        <v>1588</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A95" s="13" t="s">
+        <v>781</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>1569</v>
+        <v>1564</v>
       </c>
       <c r="D95" s="7" t="s">
         <v>1567</v>
@@ -10561,769 +10592,829 @@
       <c r="E95" s="8">
         <v>300014109</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G95" s="12" t="s">
+        <v>1587</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A96" s="6" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="C96" s="6" t="s">
         <v>1569</v>
       </c>
       <c r="D96" s="7" t="s">
-        <v>1579</v>
+        <v>1567</v>
       </c>
       <c r="E96" s="8">
-        <v>300027354</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+        <v>300014109</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A97" s="6" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>790</v>
-      </c>
-      <c r="F97" s="6" t="s">
-        <v>1329</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+        <v>786</v>
+      </c>
+      <c r="C97" s="6" t="s">
+        <v>1569</v>
+      </c>
+      <c r="D97" s="7" t="s">
+        <v>1567</v>
+      </c>
+      <c r="E97" s="8">
+        <v>300014109</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="6" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="C98" s="6" t="s">
         <v>1569</v>
       </c>
       <c r="D98" s="7" t="s">
+        <v>1579</v>
+      </c>
+      <c r="E98" s="8">
+        <v>300027354</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A99" s="6" t="s">
+        <v>789</v>
+      </c>
+      <c r="B99" s="6" t="s">
+        <v>790</v>
+      </c>
+      <c r="F99" s="6" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A100" s="6" t="s">
+        <v>791</v>
+      </c>
+      <c r="B100" s="6" t="s">
+        <v>792</v>
+      </c>
+      <c r="C100" s="6" t="s">
+        <v>1569</v>
+      </c>
+      <c r="D100" s="7" t="s">
         <v>1580</v>
       </c>
-      <c r="E98" s="8">
+      <c r="E100" s="8">
         <v>300014206</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A99" s="6" t="s">
+    <row r="101" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A101" s="6" t="s">
         <v>793</v>
       </c>
-      <c r="B99" s="6" t="s">
+      <c r="B101" s="6" t="s">
         <v>683</v>
-      </c>
-      <c r="C99" s="6" t="s">
-        <v>1564</v>
-      </c>
-      <c r="D99" s="7" t="s">
-        <v>1517</v>
-      </c>
-      <c r="E99" s="14">
-        <v>300011176</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A100" s="6" t="s">
-        <v>794</v>
-      </c>
-      <c r="B100" s="6" t="s">
-        <v>795</v>
-      </c>
-      <c r="C100" s="6" t="s">
-        <v>1564</v>
-      </c>
-      <c r="D100" s="7" t="s">
-        <v>1544</v>
-      </c>
-      <c r="E100" s="8">
-        <v>300010900</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A101" s="6" t="s">
-        <v>796</v>
-      </c>
-      <c r="B101" s="6" t="s">
-        <v>797</v>
       </c>
       <c r="C101" s="6" t="s">
         <v>1564</v>
       </c>
       <c r="D101" s="7" t="s">
-        <v>1559</v>
-      </c>
-      <c r="E101" s="8">
-        <v>300014248</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1517</v>
+      </c>
+      <c r="E101" s="14">
+        <v>300011176</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" s="6" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>1569</v>
+        <v>1564</v>
       </c>
       <c r="D102" s="7" t="s">
-        <v>1581</v>
+        <v>1544</v>
       </c>
       <c r="E102" s="8">
-        <v>300012849</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+        <v>300010900</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" s="6" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
       <c r="C103" s="6" t="s">
         <v>1564</v>
       </c>
       <c r="D103" s="7" t="s">
-        <v>1535</v>
+        <v>1559</v>
       </c>
       <c r="E103" s="8">
-        <v>300231565</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+        <v>300014248</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" s="6" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="C104" s="6" t="s">
         <v>1569</v>
       </c>
       <c r="D104" s="7" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
       <c r="E104" s="8">
-        <v>300014203</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+        <v>300012849</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A105" s="6" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>690</v>
-      </c>
-      <c r="F105" s="6" t="s">
-        <v>1329</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+        <v>801</v>
+      </c>
+      <c r="C105" s="6" t="s">
+        <v>1564</v>
+      </c>
+      <c r="D105" s="7" t="s">
+        <v>1535</v>
+      </c>
+      <c r="E105" s="8">
+        <v>300231565</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" s="6" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="C106" s="6" t="s">
         <v>1569</v>
       </c>
       <c r="D106" s="7" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="E106" s="8">
-        <v>300014184</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+        <v>300014203</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" s="6" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>646</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+        <v>690</v>
+      </c>
+      <c r="F107" s="6" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" s="6" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>700</v>
+        <v>806</v>
       </c>
       <c r="C108" s="6" t="s">
         <v>1569</v>
       </c>
       <c r="D108" s="7" t="s">
-        <v>1585</v>
+        <v>1583</v>
       </c>
       <c r="E108" s="8">
-        <v>300011037</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+        <v>300014184</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="6" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>698</v>
-      </c>
-      <c r="C109" s="6" t="s">
-        <v>1564</v>
-      </c>
-      <c r="D109" s="7" t="s">
-        <v>1563</v>
-      </c>
-      <c r="E109" s="8">
-        <v>300231565</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" s="6" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>811</v>
+        <v>700</v>
       </c>
       <c r="C110" s="6" t="s">
         <v>1569</v>
       </c>
       <c r="D110" s="7" t="s">
-        <v>1584</v>
+        <v>1585</v>
       </c>
       <c r="E110" s="8">
-        <v>300243428</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+        <v>300011037</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A111" s="6" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>813</v>
+        <v>698</v>
       </c>
       <c r="C111" s="6" t="s">
         <v>1564</v>
       </c>
       <c r="D111" s="7" t="s">
-        <v>1538</v>
+        <v>1563</v>
       </c>
       <c r="E111" s="8">
-        <v>300022453</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A112" s="6" t="s">
-        <v>814</v>
+        <v>300231565</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A112" s="13" t="s">
+        <v>810</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>1460</v>
-      </c>
-      <c r="D112" s="6" t="s">
-        <v>1469</v>
-      </c>
-      <c r="E112" s="6">
-        <v>300138699</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A113" s="6" t="s">
-        <v>816</v>
+        <v>1569</v>
+      </c>
+      <c r="D112" s="7" t="s">
+        <v>1584</v>
+      </c>
+      <c r="E112" s="8">
+        <v>300243428</v>
+      </c>
+      <c r="G112" s="11" t="s">
+        <v>1570</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A113" s="13" t="s">
+        <v>810</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>817</v>
+        <v>811</v>
       </c>
       <c r="C113" s="6" t="s">
         <v>1564</v>
       </c>
       <c r="D113" s="7" t="s">
-        <v>1521</v>
+        <v>1584</v>
       </c>
       <c r="E113" s="8">
-        <v>300011729</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+        <v>300243428</v>
+      </c>
+      <c r="G113" s="12" t="s">
+        <v>1530</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" s="6" t="s">
-        <v>818</v>
+        <v>812</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>819</v>
+        <v>813</v>
       </c>
       <c r="C114" s="6" t="s">
+        <v>1564</v>
+      </c>
+      <c r="D114" s="7" t="s">
+        <v>1538</v>
+      </c>
+      <c r="E114" s="8">
+        <v>300022453</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A115" s="6" t="s">
+        <v>814</v>
+      </c>
+      <c r="B115" s="6" t="s">
+        <v>815</v>
+      </c>
+      <c r="C115" s="6" t="s">
         <v>1460</v>
       </c>
-      <c r="D114" s="7" t="s">
-        <v>1483</v>
-      </c>
-      <c r="E114" s="8">
-        <v>300179099</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A115" s="6" t="s">
-        <v>820</v>
-      </c>
-      <c r="B115" s="6" t="s">
-        <v>821</v>
-      </c>
-      <c r="C115" s="6" t="s">
-        <v>1564</v>
-      </c>
-      <c r="D115" s="7" t="s">
-        <v>1531</v>
-      </c>
-      <c r="E115" s="8">
-        <v>300012862</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D115" s="6" t="s">
+        <v>1469</v>
+      </c>
+      <c r="E115" s="6">
+        <v>300138699</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A116" s="6" t="s">
-        <v>822</v>
+        <v>816</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>823</v>
+        <v>817</v>
       </c>
       <c r="C116" s="6" t="s">
         <v>1564</v>
       </c>
       <c r="D116" s="7" t="s">
-        <v>1533</v>
+        <v>1521</v>
       </c>
       <c r="E116" s="8">
-        <v>300015012</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+        <v>300011729</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A117" s="6" t="s">
-        <v>824</v>
+        <v>818</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>825</v>
+        <v>819</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>1564</v>
+        <v>1460</v>
       </c>
       <c r="D117" s="7" t="s">
-        <v>1536</v>
+        <v>1483</v>
       </c>
       <c r="E117" s="8">
-        <v>300022413</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+        <v>300179099</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A118" s="6" t="s">
-        <v>826</v>
+        <v>820</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>827</v>
+        <v>821</v>
       </c>
       <c r="C118" s="6" t="s">
         <v>1564</v>
       </c>
       <c r="D118" s="7" t="s">
-        <v>1537</v>
+        <v>1531</v>
       </c>
       <c r="E118" s="8">
-        <v>300022441</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+        <v>300012862</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" s="6" t="s">
-        <v>828</v>
+        <v>822</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>829</v>
+        <v>823</v>
       </c>
       <c r="C119" s="6" t="s">
         <v>1564</v>
       </c>
       <c r="D119" s="7" t="s">
+        <v>1533</v>
+      </c>
+      <c r="E119" s="8">
+        <v>300015012</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A120" s="6" t="s">
+        <v>824</v>
+      </c>
+      <c r="B120" s="6" t="s">
+        <v>825</v>
+      </c>
+      <c r="C120" s="6" t="s">
+        <v>1564</v>
+      </c>
+      <c r="D120" s="7" t="s">
         <v>1536</v>
       </c>
-      <c r="E119" s="8">
+      <c r="E120" s="8">
         <v>300022413</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A120" s="6" t="s">
-        <v>830</v>
-      </c>
-      <c r="B120" s="6" t="s">
-        <v>831</v>
-      </c>
-      <c r="C120" s="6" t="s">
-        <v>1460</v>
-      </c>
-      <c r="D120" s="6" t="s">
-        <v>1503</v>
-      </c>
-      <c r="E120" s="6">
-        <v>300053277</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A121" s="6" t="s">
-        <v>832</v>
+        <v>826</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>833</v>
+        <v>827</v>
       </c>
       <c r="C121" s="6" t="s">
         <v>1564</v>
       </c>
       <c r="D121" s="7" t="s">
-        <v>1547</v>
+        <v>1537</v>
       </c>
       <c r="E121" s="8">
-        <v>300022439</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+        <v>300022441</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" s="6" t="s">
-        <v>834</v>
+        <v>828</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>835</v>
+        <v>829</v>
       </c>
       <c r="C122" s="6" t="s">
         <v>1564</v>
       </c>
       <c r="D122" s="7" t="s">
-        <v>1550</v>
+        <v>1536</v>
       </c>
       <c r="E122" s="8">
-        <v>300015018</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+        <v>300022413</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" s="6" t="s">
-        <v>836</v>
+        <v>830</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="C123" s="6" t="s">
-        <v>1564</v>
-      </c>
-      <c r="D123" s="7" t="s">
-        <v>1548</v>
-      </c>
-      <c r="E123" s="8">
-        <v>300230810</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+        <v>1460</v>
+      </c>
+      <c r="D123" s="6" t="s">
+        <v>1503</v>
+      </c>
+      <c r="E123" s="6">
+        <v>300053277</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A124" s="6" t="s">
-        <v>838</v>
+        <v>832</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>839</v>
+        <v>833</v>
       </c>
       <c r="C124" s="6" t="s">
         <v>1564</v>
       </c>
       <c r="D124" s="7" t="s">
-        <v>1550</v>
+        <v>1547</v>
       </c>
       <c r="E124" s="8">
-        <v>300015018</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+        <v>300022439</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A125" s="6" t="s">
-        <v>840</v>
+        <v>834</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>841</v>
+        <v>835</v>
       </c>
       <c r="C125" s="6" t="s">
         <v>1564</v>
       </c>
       <c r="D125" s="7" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="E125" s="8">
-        <v>300122621</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+        <v>300015018</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126" s="6" t="s">
-        <v>842</v>
+        <v>836</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>843</v>
+        <v>837</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>1460</v>
-      </c>
-      <c r="D126" s="6" t="s">
-        <v>1505</v>
-      </c>
-      <c r="E126" s="6">
-        <v>300022452</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
+        <v>1564</v>
+      </c>
+      <c r="D126" s="7" t="s">
+        <v>1548</v>
+      </c>
+      <c r="E126" s="8">
+        <v>300230810</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A127" s="6" t="s">
-        <v>844</v>
+        <v>838</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>845</v>
+        <v>839</v>
       </c>
       <c r="C127" s="6" t="s">
         <v>1564</v>
       </c>
       <c r="D127" s="7" t="s">
-        <v>1547</v>
+        <v>1550</v>
       </c>
       <c r="E127" s="8">
-        <v>300022439</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+        <v>300015018</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A128" s="6" t="s">
-        <v>846</v>
+        <v>840</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>847</v>
+        <v>841</v>
       </c>
       <c r="C128" s="6" t="s">
-        <v>1460</v>
-      </c>
-      <c r="D128" s="6" t="s">
-        <v>1506</v>
-      </c>
-      <c r="E128" s="6">
-        <v>300022552</v>
+        <v>1564</v>
+      </c>
+      <c r="D128" s="7" t="s">
+        <v>1551</v>
+      </c>
+      <c r="E128" s="8">
+        <v>300122621</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" s="6" t="s">
-        <v>848</v>
+        <v>842</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>849</v>
+        <v>843</v>
       </c>
       <c r="C129" s="6" t="s">
-        <v>1564</v>
-      </c>
-      <c r="D129" s="7" t="s">
-        <v>1533</v>
-      </c>
-      <c r="E129" s="8">
-        <v>300015012</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1460</v>
+      </c>
+      <c r="D129" s="6" t="s">
+        <v>1505</v>
+      </c>
+      <c r="E129" s="6">
+        <v>300022452</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A130" s="6" t="s">
-        <v>850</v>
+        <v>844</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>600</v>
+        <v>845</v>
       </c>
       <c r="C130" s="6" t="s">
         <v>1564</v>
       </c>
       <c r="D130" s="7" t="s">
-        <v>1555</v>
+        <v>1547</v>
       </c>
       <c r="E130" s="8">
-        <v>300080064</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+        <v>300022439</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" s="6" t="s">
-        <v>851</v>
+        <v>846</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>852</v>
+        <v>847</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>1564</v>
-      </c>
-      <c r="D131" s="7" t="s">
-        <v>1496</v>
-      </c>
-      <c r="E131" s="8">
-        <v>300417481</v>
+        <v>1460</v>
+      </c>
+      <c r="D131" s="6" t="s">
+        <v>1506</v>
+      </c>
+      <c r="E131" s="6">
+        <v>300022552</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132" s="6" t="s">
-        <v>853</v>
+        <v>848</v>
       </c>
       <c r="B132" s="6" t="s">
-        <v>854</v>
+        <v>849</v>
       </c>
       <c r="C132" s="6" t="s">
         <v>1564</v>
       </c>
       <c r="D132" s="7" t="s">
-        <v>1560</v>
+        <v>1533</v>
       </c>
       <c r="E132" s="8">
-        <v>300022458</v>
+        <v>300015012</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" s="6" t="s">
-        <v>855</v>
+        <v>850</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>856</v>
+        <v>600</v>
       </c>
       <c r="C133" s="6" t="s">
         <v>1564</v>
       </c>
       <c r="D133" s="7" t="s">
-        <v>1562</v>
+        <v>1555</v>
       </c>
       <c r="E133" s="8">
-        <v>300167812</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+        <v>300080064</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A134" s="6" t="s">
-        <v>857</v>
+        <v>851</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>858</v>
-      </c>
-      <c r="F134" s="6" t="s">
-        <v>1329</v>
+        <v>852</v>
+      </c>
+      <c r="C134" s="6" t="s">
+        <v>1564</v>
+      </c>
+      <c r="D134" s="7" t="s">
+        <v>1496</v>
+      </c>
+      <c r="E134" s="8">
+        <v>300417481</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135" s="6" t="s">
-        <v>859</v>
+        <v>853</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>860</v>
-      </c>
-      <c r="F135" s="6" t="s">
-        <v>1329</v>
+        <v>854</v>
+      </c>
+      <c r="C135" s="6" t="s">
+        <v>1564</v>
+      </c>
+      <c r="D135" s="7" t="s">
+        <v>1560</v>
+      </c>
+      <c r="E135" s="8">
+        <v>300022458</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136" s="6" t="s">
-        <v>861</v>
+        <v>855</v>
       </c>
       <c r="B136" s="6" t="s">
-        <v>862</v>
+        <v>856</v>
       </c>
       <c r="C136" s="6" t="s">
-        <v>1460</v>
+        <v>1564</v>
       </c>
       <c r="D136" s="7" t="s">
-        <v>1482</v>
+        <v>1562</v>
       </c>
       <c r="E136" s="8">
-        <v>300053796</v>
+        <v>300167812</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" s="6" t="s">
-        <v>863</v>
+        <v>857</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>864</v>
+        <v>858</v>
       </c>
       <c r="F137" s="6" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="138" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138" s="6" t="s">
-        <v>865</v>
+        <v>859</v>
       </c>
       <c r="B138" s="6" t="s">
-        <v>866</v>
-      </c>
-      <c r="C138" s="6" t="s">
-        <v>1460</v>
-      </c>
-      <c r="D138" s="7" t="s">
-        <v>1478</v>
-      </c>
-      <c r="E138" s="8">
-        <v>300311416</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+        <v>860</v>
+      </c>
+      <c r="F138" s="6" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" s="6" t="s">
-        <v>867</v>
+        <v>861</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>868</v>
+        <v>862</v>
       </c>
       <c r="C139" s="6" t="s">
         <v>1460</v>
       </c>
       <c r="D139" s="7" t="s">
-        <v>1485</v>
+        <v>1482</v>
       </c>
       <c r="E139" s="8">
-        <v>300054216</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+        <v>300053796</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" s="6" t="s">
-        <v>869</v>
+        <v>863</v>
       </c>
       <c r="B140" s="6" t="s">
-        <v>870</v>
-      </c>
-      <c r="C140" s="6" t="s">
-        <v>1460</v>
-      </c>
-      <c r="D140" s="7" t="s">
-        <v>1484</v>
-      </c>
-      <c r="E140" s="8">
-        <v>300443550</v>
+        <v>864</v>
+      </c>
+      <c r="F140" s="6" t="s">
+        <v>1329</v>
       </c>
     </row>
     <row r="141" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A141" s="6" t="s">
-        <v>871</v>
+        <v>865</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>872</v>
+        <v>866</v>
       </c>
       <c r="C141" s="6" t="s">
         <v>1460</v>
       </c>
       <c r="D141" s="7" t="s">
-        <v>1484</v>
+        <v>1478</v>
       </c>
       <c r="E141" s="8">
-        <v>300443550</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+        <v>300311416</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A142" s="6" t="s">
-        <v>873</v>
+        <v>867</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>874</v>
+        <v>868</v>
       </c>
       <c r="C142" s="6" t="s">
         <v>1460</v>
       </c>
       <c r="D142" s="7" t="s">
+        <v>1485</v>
+      </c>
+      <c r="E142" s="8">
+        <v>300054216</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A143" s="6" t="s">
+        <v>869</v>
+      </c>
+      <c r="B143" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="C143" s="6" t="s">
+        <v>1460</v>
+      </c>
+      <c r="D143" s="7" t="s">
+        <v>1484</v>
+      </c>
+      <c r="E143" s="8">
+        <v>300443550</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A144" s="6" t="s">
+        <v>871</v>
+      </c>
+      <c r="B144" s="6" t="s">
+        <v>872</v>
+      </c>
+      <c r="C144" s="6" t="s">
+        <v>1460</v>
+      </c>
+      <c r="D144" s="7" t="s">
+        <v>1484</v>
+      </c>
+      <c r="E144" s="8">
+        <v>300443550</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A145" s="6" t="s">
+        <v>873</v>
+      </c>
+      <c r="B145" s="6" t="s">
+        <v>874</v>
+      </c>
+      <c r="C145" s="6" t="s">
+        <v>1460</v>
+      </c>
+      <c r="D145" s="7" t="s">
         <v>1510</v>
       </c>
-      <c r="E142" s="8">
+      <c r="E145" s="8">
         <v>300053989</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F142"/>
+  <autoFilter ref="A1:F145"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -11337,8 +11428,8 @@
   <dimension ref="A1:F162"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -13508,7 +13599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Digipolis Thesauri\Schrijfstadium Type -> Digipolis Thesauri\Productiestadium Type
</commit_message>
<xml_diff>
--- a/admin/rdm/Digipolis_Lookup_RDM_Cleaning.xlsx
+++ b/admin/rdm/Digipolis_Lookup_RDM_Cleaning.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="24" yWindow="456" windowWidth="28404" windowHeight="17040" firstSheet="13" activeTab="15"/>
+    <workbookView xWindow="24" yWindow="456" windowWidth="28404" windowHeight="17040" firstSheet="11" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="CSV &lt;-&gt; RDM" sheetId="25" r:id="rId1"/>
@@ -69,18 +69,10 @@
     <definedName name="toegang_types" localSheetId="25">toegang_types.csv!$A$1:$B$2</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -5421,9 +5413,6 @@
     <t>transcriptions (documents)</t>
   </si>
   <si>
-    <t>Digipolis Thesauri\Schrijfstadium Type\</t>
-  </si>
-  <si>
     <t>handwriting</t>
   </si>
   <si>
@@ -5476,6 +5465,9 @@
   </si>
   <si>
     <t>photograph albums (albums (books)</t>
+  </si>
+  <si>
+    <t>Digipolis Thesauri\Productiestadium Type\</t>
   </si>
 </sst>
 </file>
@@ -6514,9 +6506,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C53" sqref="C53:E53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -7005,7 +6997,7 @@
         <v>215</v>
       </c>
       <c r="C29" t="s">
-        <v>1706</v>
+        <v>1724</v>
       </c>
       <c r="D29" t="s">
         <v>1614</v>
@@ -7370,7 +7362,7 @@
         <v>1445</v>
       </c>
       <c r="D51" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
       <c r="E51">
         <v>300252927</v>
@@ -7387,7 +7379,7 @@
         <v>1445</v>
       </c>
       <c r="D52" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="E52">
         <v>300247929</v>
@@ -7404,7 +7396,7 @@
         <v>1445</v>
       </c>
       <c r="D53" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="E53">
         <v>300053319</v>
@@ -7537,7 +7529,7 @@
         <v>1445</v>
       </c>
       <c r="D61" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="E61">
         <v>300247929</v>
@@ -7554,7 +7546,7 @@
         <v>1701</v>
       </c>
       <c r="D62" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -7568,7 +7560,7 @@
         <v>1701</v>
       </c>
       <c r="D63" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
@@ -7582,7 +7574,7 @@
         <v>1701</v>
       </c>
       <c r="D64" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -7664,7 +7656,7 @@
         <v>1445</v>
       </c>
       <c r="D70" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="E70">
         <v>300053319</v>
@@ -7681,7 +7673,7 @@
         <v>1445</v>
       </c>
       <c r="D71" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="E71">
         <v>300374824</v>
@@ -8158,10 +8150,10 @@
         <v>349</v>
       </c>
       <c r="C2" t="s">
+        <v>1713</v>
+      </c>
+      <c r="D2" t="s">
         <v>1714</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1715</v>
       </c>
       <c r="E2">
         <v>300128366</v>
@@ -8175,10 +8167,10 @@
         <v>351</v>
       </c>
       <c r="C3" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="D3" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
       <c r="E3">
         <v>300128357</v>
@@ -8192,10 +8184,10 @@
         <v>353</v>
       </c>
       <c r="C4" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="D4" t="s">
-        <v>1717</v>
+        <v>1716</v>
       </c>
       <c r="E4">
         <v>300128359</v>
@@ -8209,10 +8201,10 @@
         <v>355</v>
       </c>
       <c r="C5" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="D5" t="s">
-        <v>1718</v>
+        <v>1717</v>
       </c>
       <c r="E5">
         <v>300127181</v>
@@ -8226,7 +8218,7 @@
         <v>357</v>
       </c>
       <c r="C6" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -8237,10 +8229,10 @@
         <v>359</v>
       </c>
       <c r="C7" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="D7" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
       <c r="E7">
         <v>300265083</v>
@@ -8254,10 +8246,10 @@
         <v>361</v>
       </c>
       <c r="C8" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="D8" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="E8">
         <v>300115233</v>
@@ -8271,10 +8263,10 @@
         <v>363</v>
       </c>
       <c r="C9" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="D9" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="E9">
         <v>300128374</v>
@@ -8288,10 +8280,10 @@
         <v>365</v>
       </c>
       <c r="C10" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="D10" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="E10">
         <v>300128343</v>
@@ -8305,10 +8297,10 @@
         <v>367</v>
       </c>
       <c r="C11" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="D11" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
       <c r="E11">
         <v>300128347</v>
@@ -8316,10 +8308,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="D12" t="s">
-        <v>1724</v>
+        <v>1723</v>
       </c>
       <c r="E12">
         <v>300026695</v>
@@ -8334,7 +8326,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -8813,7 +8805,7 @@
         <v>1674</v>
       </c>
       <c r="E28" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="F28">
         <v>300264330</v>
@@ -9582,7 +9574,7 @@
         <v>1438</v>
       </c>
       <c r="D28" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="E28">
         <v>300386629</v>
@@ -10401,7 +10393,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>615</v>
       </c>
@@ -10418,7 +10410,7 @@
         <v>300011015</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>617</v>
       </c>
@@ -10435,7 +10427,7 @@
         <v>300011176</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>619</v>
       </c>
@@ -10542,7 +10534,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>635</v>
       </c>
@@ -10559,7 +10551,7 @@
         <v>300011176</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>637</v>
       </c>
@@ -10632,7 +10624,7 @@
         <v>300011002</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>647</v>
       </c>
@@ -10649,7 +10641,7 @@
         <v>300011857</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>649</v>
       </c>
@@ -10666,7 +10658,7 @@
         <v>300235507</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>651</v>
       </c>
@@ -10683,7 +10675,7 @@
         <v>300011020</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>653</v>
       </c>
@@ -10728,7 +10720,7 @@
         <v>300011914</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>659</v>
       </c>
@@ -10745,7 +10737,7 @@
         <v>300011443</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>661</v>
       </c>
@@ -10773,7 +10765,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>665</v>
       </c>
@@ -10790,7 +10782,7 @@
         <v>300163347</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>667</v>
       </c>
@@ -10841,7 +10833,7 @@
         <v>300011914</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>673</v>
       </c>
@@ -10858,7 +10850,7 @@
         <v>300014436</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
         <v>675</v>
       </c>
@@ -10875,7 +10867,7 @@
         <v>300014546</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
         <v>676</v>
       </c>
@@ -10892,7 +10884,7 @@
         <v>300010662</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>678</v>
       </c>
@@ -10926,7 +10918,7 @@
         <v>300010822</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
         <v>682</v>
       </c>
@@ -10954,7 +10946,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>686</v>
       </c>
@@ -11016,7 +11008,7 @@
         <v>300014585</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
         <v>693</v>
       </c>
@@ -11033,7 +11025,7 @@
         <v>300011176</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
         <v>695</v>
       </c>
@@ -11050,7 +11042,7 @@
         <v>300011176</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
         <v>697</v>
       </c>
@@ -11089,7 +11081,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
         <v>703</v>
       </c>
@@ -11117,7 +11109,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>707</v>
       </c>
@@ -11145,7 +11137,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="6" t="s">
         <v>711</v>
       </c>
@@ -11162,7 +11154,7 @@
         <v>300010957</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="140.4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A53" s="11" t="s">
         <v>712</v>
       </c>
@@ -11182,7 +11174,7 @@
         <v>1515</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
         <v>713</v>
       </c>
@@ -11199,7 +11191,7 @@
         <v>300014078</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
         <v>715</v>
       </c>
@@ -11233,7 +11225,7 @@
         <v>1550</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A57" s="6" t="s">
         <v>719</v>
       </c>
@@ -11250,7 +11242,7 @@
         <v>300014910</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
         <v>721</v>
       </c>
@@ -11278,7 +11270,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="6" t="s">
         <v>725</v>
       </c>
@@ -11329,7 +11321,7 @@
         <v>300014109</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="156" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A63" s="13" t="s">
         <v>731</v>
       </c>
@@ -11349,7 +11341,7 @@
         <v>1511</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="13" t="s">
         <v>731</v>
       </c>
@@ -11386,7 +11378,7 @@
         <v>300011914</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="140.4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="13" t="s">
         <v>734</v>
       </c>
@@ -11426,7 +11418,7 @@
         <v>1555</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="6" t="s">
         <v>735</v>
       </c>
@@ -11451,7 +11443,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A70" s="6" t="s">
         <v>738</v>
       </c>
@@ -11468,7 +11460,7 @@
         <v>300014143</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
         <v>740</v>
       </c>
@@ -11485,7 +11477,7 @@
         <v>300231565</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A72" s="6" t="s">
         <v>742</v>
       </c>
@@ -11502,7 +11494,7 @@
         <v>300435274</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="6" t="s">
         <v>744</v>
       </c>
@@ -11593,7 +11585,7 @@
         <v>300014570</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="6" t="s">
         <v>751</v>
       </c>
@@ -11627,7 +11619,7 @@
         <v>300011845</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="6" t="s">
         <v>755</v>
       </c>
@@ -11678,7 +11670,7 @@
         <v>300014109</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="6" t="s">
         <v>761</v>
       </c>
@@ -11698,7 +11690,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A84" s="6" t="s">
         <v>762</v>
       </c>
@@ -11754,7 +11746,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A88" s="6" t="s">
         <v>769</v>
       </c>
@@ -11771,7 +11763,7 @@
         <v>300014657</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A89" s="6" t="s">
         <v>771</v>
       </c>
@@ -11822,7 +11814,7 @@
         <v>300014109</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A92" s="6" t="s">
         <v>777</v>
       </c>
@@ -11839,7 +11831,7 @@
         <v>300011851</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="6" t="s">
         <v>779</v>
       </c>
@@ -11958,7 +11950,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="6" t="s">
         <v>791</v>
       </c>
@@ -11975,7 +11967,7 @@
         <v>300014206</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="6" t="s">
         <v>793</v>
       </c>
@@ -12043,7 +12035,7 @@
         <v>300012849</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" s="6" t="s">
         <v>800</v>
       </c>
@@ -12130,7 +12122,7 @@
         <v>300011037</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" s="6" t="s">
         <v>809</v>
       </c>
@@ -12221,7 +12213,7 @@
         <v>300138699</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" s="6" t="s">
         <v>816</v>
       </c>
@@ -12238,7 +12230,7 @@
         <v>300011729</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" s="6" t="s">
         <v>818</v>
       </c>
@@ -12255,7 +12247,7 @@
         <v>300179099</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" s="6" t="s">
         <v>820</v>
       </c>
@@ -12306,7 +12298,7 @@
         <v>300022413</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" s="6" t="s">
         <v>826</v>
       </c>
@@ -12357,7 +12349,7 @@
         <v>300053277</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A124" s="6" t="s">
         <v>832</v>
       </c>
@@ -12374,7 +12366,7 @@
         <v>300022439</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125" s="6" t="s">
         <v>834</v>
       </c>
@@ -12408,7 +12400,7 @@
         <v>300230810</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127" s="6" t="s">
         <v>838</v>
       </c>
@@ -12425,7 +12417,7 @@
         <v>300015018</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128" s="6" t="s">
         <v>840</v>
       </c>
@@ -12459,7 +12451,7 @@
         <v>300022452</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A130" s="6" t="s">
         <v>844</v>
       </c>
@@ -12527,7 +12519,7 @@
         <v>300080064</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134" s="6" t="s">
         <v>851</v>
       </c>
@@ -12651,7 +12643,7 @@
         <v>300311416</v>
       </c>
     </row>
-    <row r="142" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A142" s="6" t="s">
         <v>867</v>
       </c>
@@ -12668,7 +12660,7 @@
         <v>300054216</v>
       </c>
     </row>
-    <row r="143" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" s="6" t="s">
         <v>869</v>
       </c>
@@ -12685,7 +12677,7 @@
         <v>300443550</v>
       </c>
     </row>
-    <row r="144" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" s="6" t="s">
         <v>871</v>
       </c>

</xml_diff>

<commit_message>
changed mappings in titel_types.csv
TODO: beschrijving_types.csv (first figure out how Beschrijving Type can be removed and documented in the mapping)
</commit_message>
<xml_diff>
--- a/admin/rdm/Digipolis_Lookup_RDM_Cleaning.xlsx
+++ b/admin/rdm/Digipolis_Lookup_RDM_Cleaning.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="24" yWindow="456" windowWidth="28404" windowHeight="17040" activeTab="1"/>
+    <workbookView xWindow="24" yWindow="456" windowWidth="28404" windowHeight="17040" firstSheet="21" activeTab="25"/>
   </bookViews>
   <sheets>
     <sheet name="CSV &lt;-&gt; RDM" sheetId="25" r:id="rId1"/>
@@ -285,7 +285,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5525" uniqueCount="1739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5525" uniqueCount="1740">
   <si>
     <t>code</t>
   </si>
@@ -5511,6 +5511,9 @@
   </si>
   <si>
     <t>prints (visual works)</t>
+  </si>
+  <si>
+    <t>constructed titles</t>
   </si>
 </sst>
 </file>
@@ -10574,8 +10577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G679"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A460" workbookViewId="0">
+      <selection activeCell="C463" sqref="C463:E463"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -11395,7 +11398,7 @@
       </c>
       <c r="G45" s="21"/>
     </row>
-    <row r="46" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="21" t="s">
         <v>484</v>
       </c>
@@ -11403,13 +11406,13 @@
         <v>1092</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>1395</v>
+        <v>1399</v>
       </c>
       <c r="D46" s="22" t="s">
-        <v>1359</v>
+        <v>1739</v>
       </c>
       <c r="E46" s="23">
-        <v>300435416</v>
+        <v>300417205</v>
       </c>
       <c r="F46" s="22"/>
       <c r="G46" s="21"/>
@@ -18984,7 +18987,7 @@
       <c r="F462" s="22"/>
       <c r="G462" s="22"/>
     </row>
-    <row r="463" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="463" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A463" s="21" t="s">
         <v>1097</v>
       </c>
@@ -18992,13 +18995,13 @@
         <v>1098</v>
       </c>
       <c r="C463" s="22" t="s">
-        <v>1395</v>
+        <v>1399</v>
       </c>
       <c r="D463" s="22" t="s">
-        <v>1359</v>
+        <v>1739</v>
       </c>
       <c r="E463" s="23">
-        <v>300435416</v>
+        <v>300417205</v>
       </c>
       <c r="F463" s="22"/>
       <c r="G463" s="21"/>
@@ -27606,8 +27609,8 @@
   </sheetPr>
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -27646,13 +27649,13 @@
         <v>1092</v>
       </c>
       <c r="C2" t="s">
-        <v>1395</v>
+        <v>1399</v>
       </c>
       <c r="D2" t="s">
-        <v>1359</v>
+        <v>1739</v>
       </c>
       <c r="E2">
-        <v>300435416</v>
+        <v>300417205</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -27714,13 +27717,13 @@
         <v>1098</v>
       </c>
       <c r="C6" t="s">
-        <v>1395</v>
+        <v>1399</v>
       </c>
       <c r="D6" t="s">
-        <v>1359</v>
+        <v>1739</v>
       </c>
       <c r="E6">
-        <v>300435416</v>
+        <v>300417205</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
added Digipolis Thesauri\ISAAR Relatie Type\	representation (form of expression)	300069747
</commit_message>
<xml_diff>
--- a/admin/rdm/Digipolis_Lookup_RDM_Cleaning.xlsx
+++ b/admin/rdm/Digipolis_Lookup_RDM_Cleaning.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="24" yWindow="456" windowWidth="28404" windowHeight="17040" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="24" yWindow="456" windowWidth="28404" windowHeight="17040" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CSV &lt;-&gt; RDM" sheetId="25" r:id="rId1"/>
@@ -285,7 +285,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5519" uniqueCount="1739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5525" uniqueCount="1741">
   <si>
     <t>code</t>
   </si>
@@ -5511,15 +5511,28 @@
   </si>
   <si>
     <t>constructed titles</t>
+  </si>
+  <si>
+    <t>afgebeeld op</t>
+  </si>
+  <si>
+    <t>representation (form of expression)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -5614,15 +5627,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -5642,7 +5655,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -5659,15 +5672,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -9343,10 +9357,10 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="A38" sqref="A1:E1048576"/>
+      <selection activeCell="E41" sqref="B41:E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -9998,6 +10012,20 @@
       </c>
       <c r="F40" t="s">
         <v>1329</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>1739</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D41" t="s">
+        <v>1740</v>
+      </c>
+      <c r="E41">
+        <v>300069747</v>
       </c>
     </row>
   </sheetData>
@@ -10582,13 +10610,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G678"/>
+  <dimension ref="A1:G679"/>
   <sheetViews>
-    <sheetView topLeftCell="A537" workbookViewId="0">
-      <selection activeCell="B541" sqref="B541"/>
+    <sheetView tabSelected="1" topLeftCell="A678" workbookViewId="0">
+      <selection activeCell="F678" sqref="F678"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -22935,6 +22966,20 @@
       </c>
       <c r="F678" s="22"/>
       <c r="G678" s="21"/>
+    </row>
+    <row r="679" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B679" s="25" t="s">
+        <v>1739</v>
+      </c>
+      <c r="C679" s="25" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D679" s="25" t="s">
+        <v>1740</v>
+      </c>
+      <c r="E679" s="25">
+        <v>300069747</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -30988,7 +31033,7 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed label of "paint" to "paint (coating)"
</commit_message>
<xml_diff>
--- a/admin/rdm/Digipolis_Lookup_RDM_Cleaning.xlsx
+++ b/admin/rdm/Digipolis_Lookup_RDM_Cleaning.xlsx
@@ -5510,7 +5510,7 @@
     <t>representation (form of expression)</t>
   </si>
   <si>
-    <t>paint</t>
+    <t>paint (coating)</t>
   </si>
 </sst>
 </file>
@@ -10654,8 +10654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G721"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A716" workbookViewId="0">
-      <selection activeCell="E721" sqref="E721"/>
+    <sheetView tabSelected="1" topLeftCell="A679" workbookViewId="0">
+      <selection activeCell="D685" sqref="D685"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -23101,7 +23101,7 @@
       <c r="C681" s="27" t="s">
         <v>1540</v>
       </c>
-      <c r="D681" s="27" t="s">
+      <c r="D681" s="31" t="s">
         <v>1738</v>
       </c>
       <c r="E681" s="28">
@@ -23137,7 +23137,7 @@
       <c r="C683" s="27" t="s">
         <v>1540</v>
       </c>
-      <c r="D683" s="27" t="s">
+      <c r="D683" s="31" t="s">
         <v>1738</v>
       </c>
       <c r="E683" s="28">
@@ -23173,7 +23173,7 @@
       <c r="C685" s="27" t="s">
         <v>1540</v>
       </c>
-      <c r="D685" s="27" t="s">
+      <c r="D685" s="31" t="s">
         <v>1738</v>
       </c>
       <c r="E685" s="28">
@@ -28707,7 +28707,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A180" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A204" sqref="A204"/>
+      <selection pane="bottomLeft" activeCell="D201" sqref="D201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
fixed kenmerken/lhtypeph GN to glass plate negatives	300393160
</commit_message>
<xml_diff>
--- a/admin/rdm/Digipolis_Lookup_RDM_Cleaning.xlsx
+++ b/admin/rdm/Digipolis_Lookup_RDM_Cleaning.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="24" yWindow="456" windowWidth="28404" windowHeight="17040" activeTab="1"/>
+    <workbookView xWindow="24" yWindow="456" windowWidth="28404" windowHeight="17040" firstSheet="11" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="CSV &lt;-&gt; RDM" sheetId="25" r:id="rId1"/>
@@ -5480,9 +5480,6 @@
     <t>datum vóór</t>
   </si>
   <si>
-    <t>clichés-verre (negatives)</t>
-  </si>
-  <si>
     <t>photograph albums</t>
   </si>
   <si>
@@ -5511,6 +5508,9 @@
   </si>
   <si>
     <t>paint (coating)</t>
+  </si>
+  <si>
+    <t>glass plate negatives</t>
   </si>
 </sst>
 </file>
@@ -8392,8 +8392,8 @@
   </sheetPr>
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -8512,10 +8512,10 @@
         <v>1698</v>
       </c>
       <c r="D7" t="s">
-        <v>1728</v>
+        <v>1738</v>
       </c>
       <c r="E7">
-        <v>300265083</v>
+        <v>300393160</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -8594,7 +8594,7 @@
         <v>1698</v>
       </c>
       <c r="D12" t="s">
-        <v>1729</v>
+        <v>1728</v>
       </c>
       <c r="E12">
         <v>300026695</v>
@@ -10058,13 +10058,13 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="C41" t="s">
         <v>1433</v>
       </c>
       <c r="D41" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
       <c r="E41">
         <v>300069747</v>
@@ -10654,8 +10654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G721"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A679" workbookViewId="0">
-      <selection activeCell="D685" sqref="D685"/>
+    <sheetView topLeftCell="A327" workbookViewId="0">
+      <selection activeCell="D327" sqref="D327:E327"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -11489,7 +11489,7 @@
         <v>1398</v>
       </c>
       <c r="D46" s="22" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="E46" s="23">
         <v>300417205</v>
@@ -12882,7 +12882,7 @@
       </c>
       <c r="C123" s="22"/>
       <c r="D123" s="22" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
       <c r="E123" s="23">
         <v>300435447</v>
@@ -12983,7 +12983,7 @@
         <v>300379247</v>
       </c>
       <c r="F128" s="22" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
       <c r="G128" s="22" t="s">
         <v>1135</v>
@@ -13007,7 +13007,7 @@
       </c>
       <c r="F129" s="22"/>
       <c r="G129" s="22" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
     </row>
     <row r="130" spans="1:7" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
@@ -13026,7 +13026,7 @@
       <c r="E130" s="22"/>
       <c r="F130" s="22"/>
       <c r="G130" s="22" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
     </row>
     <row r="131" spans="1:7" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
@@ -13045,7 +13045,7 @@
       <c r="E131" s="21"/>
       <c r="F131" s="22"/>
       <c r="G131" s="22" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
     </row>
     <row r="132" spans="1:7" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
@@ -13064,7 +13064,7 @@
       <c r="E132" s="21"/>
       <c r="F132" s="22"/>
       <c r="G132" s="22" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
     </row>
     <row r="133" spans="1:7" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
@@ -13085,7 +13085,7 @@
       </c>
       <c r="F133" s="22"/>
       <c r="G133" s="22" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
     </row>
     <row r="134" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -15092,7 +15092,7 @@
         <v>1576</v>
       </c>
       <c r="D241" s="22" t="s">
-        <v>1734</v>
+        <v>1733</v>
       </c>
       <c r="E241" s="23">
         <v>300041273</v>
@@ -16158,7 +16158,7 @@
       </c>
       <c r="C299" s="22"/>
       <c r="D299" s="22" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
       <c r="E299" s="23">
         <v>300435447</v>
@@ -16680,10 +16680,10 @@
         <v>1698</v>
       </c>
       <c r="D327" s="22" t="s">
-        <v>1728</v>
+        <v>1738</v>
       </c>
       <c r="E327" s="23">
-        <v>300265083</v>
+        <v>300393160</v>
       </c>
       <c r="F327" s="22"/>
       <c r="G327" s="21"/>
@@ -19078,7 +19078,7 @@
         <v>1398</v>
       </c>
       <c r="D463" s="22" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="E463" s="23">
         <v>300417205</v>
@@ -21361,7 +21361,7 @@
         <v>1053</v>
       </c>
       <c r="B588" s="22" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
       <c r="C588" s="22" t="s">
         <v>1434</v>
@@ -23066,7 +23066,7 @@
         <v>1540</v>
       </c>
       <c r="D679" s="31" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
       <c r="E679" s="33">
         <v>300015029</v>
@@ -23102,7 +23102,7 @@
         <v>1540</v>
       </c>
       <c r="D681" s="31" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
       <c r="E681" s="28">
         <v>300015029</v>
@@ -23138,7 +23138,7 @@
         <v>1540</v>
       </c>
       <c r="D683" s="31" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
       <c r="E683" s="28">
         <v>300015029</v>
@@ -23174,7 +23174,7 @@
         <v>1540</v>
       </c>
       <c r="D685" s="31" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
       <c r="E685" s="28">
         <v>300015029</v>
@@ -23695,7 +23695,7 @@
         <v>1698</v>
       </c>
       <c r="D714" s="22" t="s">
-        <v>1729</v>
+        <v>1728</v>
       </c>
       <c r="E714" s="23">
         <v>300026695</v>
@@ -23802,13 +23802,13 @@
     <row r="721" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A721" s="30"/>
       <c r="B721" s="32" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="C721" s="32" t="s">
         <v>1433</v>
       </c>
       <c r="D721" s="32" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
       <c r="E721" s="32">
         <v>300069747</v>
@@ -28006,7 +28006,7 @@
         <v>1053</v>
       </c>
       <c r="B20" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
       <c r="C20" t="s">
         <v>1434</v>
@@ -28525,7 +28525,7 @@
         <v>1398</v>
       </c>
       <c r="D2" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="E2">
         <v>300417205</v>
@@ -28593,7 +28593,7 @@
         <v>1398</v>
       </c>
       <c r="D6" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="E6">
         <v>300417205</v>
@@ -31480,7 +31480,7 @@
         <v>1540</v>
       </c>
       <c r="D201" s="6" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
       <c r="E201" s="6">
         <v>300015029</v>
@@ -31497,7 +31497,7 @@
         <v>1540</v>
       </c>
       <c r="D202" s="6" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
       <c r="E202" s="6">
         <v>300015029</v>
@@ -31514,7 +31514,7 @@
         <v>1540</v>
       </c>
       <c r="D203" s="6" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
       <c r="E203" s="6">
         <v>300015029</v>
@@ -31531,7 +31531,7 @@
         <v>1540</v>
       </c>
       <c r="D204" s="6" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
       <c r="E204" s="6">
         <v>300015029</v>

</xml_diff>

<commit_message>
documentation: removed value as for kenmerken/lhstadiumhs
</commit_message>
<xml_diff>
--- a/admin/rdm/Digipolis_Lookup_RDM_Cleaning.xlsx
+++ b/admin/rdm/Digipolis_Lookup_RDM_Cleaning.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="24" yWindow="456" windowWidth="28404" windowHeight="17040" firstSheet="11" activeTab="15"/>
+    <workbookView xWindow="24" yWindow="456" windowWidth="28404" windowHeight="17040" firstSheet="7" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="CSV &lt;-&gt; RDM" sheetId="25" r:id="rId1"/>
@@ -285,7 +285,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5861" uniqueCount="1739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5859" uniqueCount="1739">
   <si>
     <t>code</t>
   </si>
@@ -5517,9 +5517,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -5641,15 +5648,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -5669,7 +5676,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -5686,14 +5693,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -5701,27 +5714,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6760,9 +6770,9 @@
   </sheetPr>
   <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C62" sqref="C62:C64"/>
+      <selection pane="bottomLeft" activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -7571,7 +7581,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>252</v>
       </c>
@@ -7588,7 +7598,7 @@
         <v>300027240</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>254</v>
       </c>
@@ -7605,7 +7615,7 @@
         <v>300049060</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>256</v>
       </c>
@@ -7622,7 +7632,7 @@
         <v>300252927</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>258</v>
       </c>
@@ -7639,7 +7649,7 @@
         <v>300247929</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>260</v>
       </c>
@@ -7656,7 +7666,7 @@
         <v>300053319</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>262</v>
       </c>
@@ -7673,7 +7683,7 @@
         <v>300026693</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>264</v>
       </c>
@@ -7690,7 +7700,7 @@
         <v>300027489</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>266</v>
       </c>
@@ -7707,7 +7717,7 @@
         <v>300027496</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>268</v>
       </c>
@@ -7724,7 +7734,7 @@
         <v>300027045</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>270</v>
       </c>
@@ -7738,7 +7748,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>272</v>
       </c>
@@ -7755,24 +7765,18 @@
         <v>300404333</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>274</v>
       </c>
       <c r="B60" t="s">
         <v>273</v>
       </c>
-      <c r="C60" t="s">
-        <v>1687</v>
-      </c>
-      <c r="D60" t="s">
-        <v>1691</v>
-      </c>
-      <c r="E60">
-        <v>300404333</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F60" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>275</v>
       </c>
@@ -7789,7 +7793,7 @@
         <v>300247929</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>277</v>
       </c>
@@ -7803,7 +7807,7 @@
         <v>1722</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>279</v>
       </c>
@@ -7817,7 +7821,7 @@
         <v>1723</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>281</v>
       </c>
@@ -8392,7 +8396,7 @@
   </sheetPr>
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7:E7"/>
     </sheetView>
   </sheetViews>
@@ -10654,8 +10658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G721"/>
   <sheetViews>
-    <sheetView topLeftCell="A327" workbookViewId="0">
-      <selection activeCell="D327" sqref="D327:E327"/>
+    <sheetView topLeftCell="A592" workbookViewId="0">
+      <selection activeCell="B597" sqref="B597"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -11217,23 +11221,19 @@
       <c r="F30" s="22"/>
       <c r="G30" s="22"/>
     </row>
-    <row r="31" spans="1:7" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="21" t="s">
         <v>274</v>
       </c>
       <c r="B31" s="21" t="s">
         <v>273</v>
       </c>
-      <c r="C31" s="22" t="s">
-        <v>1687</v>
-      </c>
-      <c r="D31" s="22" t="s">
-        <v>1691</v>
-      </c>
-      <c r="E31" s="23">
-        <v>300404333</v>
-      </c>
-      <c r="F31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="36" t="s">
+        <v>1329</v>
+      </c>
       <c r="G31" s="21"/>
     </row>
     <row r="32" spans="1:7" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
* added missing technique / colour stuff:   -RDM: added Digipolis Thesauri\Materiaal Type\lacquer (material) (AAT 300014916)   -RDM cleaning: added material mappings to techniques
</commit_message>
<xml_diff>
--- a/admin/rdm/Digipolis_Lookup_RDM_Cleaning.xlsx
+++ b/admin/rdm/Digipolis_Lookup_RDM_Cleaning.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="24" yWindow="456" windowWidth="28404" windowHeight="17040" firstSheet="7" activeTab="12"/>
+    <workbookView xWindow="24" yWindow="456" windowWidth="28404" windowHeight="17040" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CSV &lt;-&gt; RDM" sheetId="25" r:id="rId1"/>
@@ -285,7 +285,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5859" uniqueCount="1739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5919" uniqueCount="1740">
   <si>
     <t>code</t>
   </si>
@@ -5511,6 +5511,9 @@
   </si>
   <si>
     <t>glass plate negatives</t>
+  </si>
+  <si>
+    <t>lacquer (material)</t>
   </si>
 </sst>
 </file>
@@ -6770,7 +6773,7 @@
   </sheetPr>
   <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F61" sqref="F61"/>
     </sheetView>
@@ -10656,10 +10659,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G721"/>
+  <dimension ref="A1:G729"/>
   <sheetViews>
-    <sheetView topLeftCell="A592" workbookViewId="0">
-      <selection activeCell="B597" sqref="B597"/>
+    <sheetView tabSelected="1" topLeftCell="A719" workbookViewId="0">
+      <selection activeCell="E729" sqref="E729"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -23812,6 +23815,142 @@
       </c>
       <c r="E721" s="32">
         <v>300069747</v>
+      </c>
+    </row>
+    <row r="722" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A722" t="s">
+        <v>846</v>
+      </c>
+      <c r="B722" t="s">
+        <v>847</v>
+      </c>
+      <c r="C722" t="s">
+        <v>1540</v>
+      </c>
+      <c r="D722" t="s">
+        <v>1737</v>
+      </c>
+      <c r="E722" s="32">
+        <v>300015029</v>
+      </c>
+    </row>
+    <row r="723" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A723" t="s">
+        <v>1312</v>
+      </c>
+      <c r="B723" t="s">
+        <v>1313</v>
+      </c>
+      <c r="C723" t="s">
+        <v>1540</v>
+      </c>
+      <c r="D723" t="s">
+        <v>1492</v>
+      </c>
+      <c r="E723" s="32">
+        <v>300015045</v>
+      </c>
+    </row>
+    <row r="724" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A724" t="s">
+        <v>1317</v>
+      </c>
+      <c r="B724" t="s">
+        <v>1318</v>
+      </c>
+      <c r="C724" t="s">
+        <v>1540</v>
+      </c>
+      <c r="D724" t="s">
+        <v>1492</v>
+      </c>
+      <c r="E724" s="32">
+        <v>300015045</v>
+      </c>
+    </row>
+    <row r="725" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A725" t="s">
+        <v>1323</v>
+      </c>
+      <c r="B725" t="s">
+        <v>1324</v>
+      </c>
+      <c r="C725" t="s">
+        <v>1540</v>
+      </c>
+      <c r="D725" t="s">
+        <v>1509</v>
+      </c>
+      <c r="E725" s="32">
+        <v>300015012</v>
+      </c>
+    </row>
+    <row r="726" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A726" t="s">
+        <v>846</v>
+      </c>
+      <c r="B726" t="s">
+        <v>847</v>
+      </c>
+      <c r="C726" t="s">
+        <v>1540</v>
+      </c>
+      <c r="D726" t="s">
+        <v>1737</v>
+      </c>
+      <c r="E726" s="32">
+        <v>300015029</v>
+      </c>
+    </row>
+    <row r="727" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A727" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B727" t="s">
+        <v>1315</v>
+      </c>
+      <c r="C727" t="s">
+        <v>1540</v>
+      </c>
+      <c r="D727" t="s">
+        <v>1509</v>
+      </c>
+      <c r="E727" s="32">
+        <v>300015012</v>
+      </c>
+    </row>
+    <row r="728" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A728" t="s">
+        <v>1294</v>
+      </c>
+      <c r="B728" t="s">
+        <v>862</v>
+      </c>
+      <c r="C728" t="s">
+        <v>1540</v>
+      </c>
+      <c r="D728" t="s">
+        <v>1739</v>
+      </c>
+      <c r="E728" s="32">
+        <v>300014916</v>
+      </c>
+    </row>
+    <row r="729" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A729" t="s">
+        <v>1294</v>
+      </c>
+      <c r="B729" t="s">
+        <v>862</v>
+      </c>
+      <c r="C729" t="s">
+        <v>1540</v>
+      </c>
+      <c r="D729" t="s">
+        <v>1739</v>
+      </c>
+      <c r="E729" s="32">
+        <v>300014916</v>
       </c>
     </row>
   </sheetData>
@@ -28703,11 +28842,11 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:F204"/>
+  <dimension ref="A1:F211"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A180" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D201" sqref="D201"/>
+      <pane ySplit="1" topLeftCell="A198" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A212" sqref="A212:XFD212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -31535,6 +31674,125 @@
       </c>
       <c r="E204" s="6">
         <v>300015029</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A205" s="6" t="s">
+        <v>846</v>
+      </c>
+      <c r="B205" s="6" t="s">
+        <v>847</v>
+      </c>
+      <c r="C205" s="6" t="s">
+        <v>1540</v>
+      </c>
+      <c r="D205" s="6" t="s">
+        <v>1737</v>
+      </c>
+      <c r="E205" s="6">
+        <v>300015029</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A206" s="6" t="s">
+        <v>1312</v>
+      </c>
+      <c r="B206" s="6" t="s">
+        <v>1313</v>
+      </c>
+      <c r="C206" s="6" t="s">
+        <v>1540</v>
+      </c>
+      <c r="D206" s="6" t="s">
+        <v>1492</v>
+      </c>
+      <c r="E206" s="6">
+        <v>300015045</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A207" s="6" t="s">
+        <v>1317</v>
+      </c>
+      <c r="B207" s="6" t="s">
+        <v>1318</v>
+      </c>
+      <c r="C207" s="6" t="s">
+        <v>1540</v>
+      </c>
+      <c r="D207" s="6" t="s">
+        <v>1492</v>
+      </c>
+      <c r="E207" s="6">
+        <v>300015045</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A208" s="6" t="s">
+        <v>1323</v>
+      </c>
+      <c r="B208" s="6" t="s">
+        <v>1324</v>
+      </c>
+      <c r="C208" s="6" t="s">
+        <v>1540</v>
+      </c>
+      <c r="D208" s="6" t="s">
+        <v>1509</v>
+      </c>
+      <c r="E208" s="6">
+        <v>300015012</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A209" s="6" t="s">
+        <v>846</v>
+      </c>
+      <c r="B209" s="6" t="s">
+        <v>847</v>
+      </c>
+      <c r="C209" s="6" t="s">
+        <v>1540</v>
+      </c>
+      <c r="D209" s="6" t="s">
+        <v>1737</v>
+      </c>
+      <c r="E209" s="6">
+        <v>300015029</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A210" s="6" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B210" s="6" t="s">
+        <v>1315</v>
+      </c>
+      <c r="C210" s="6" t="s">
+        <v>1540</v>
+      </c>
+      <c r="D210" s="6" t="s">
+        <v>1509</v>
+      </c>
+      <c r="E210" s="6">
+        <v>300015012</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A211" s="6" t="s">
+        <v>1294</v>
+      </c>
+      <c r="B211" s="6" t="s">
+        <v>862</v>
+      </c>
+      <c r="C211" s="6" t="s">
+        <v>1540</v>
+      </c>
+      <c r="D211" s="6" t="s">
+        <v>1739</v>
+      </c>
+      <c r="E211" s="6">
+        <v>300014916</v>
       </c>
     </row>
   </sheetData>

</xml_diff>